<commit_message>
Updates to international fuel price data
</commit_message>
<xml_diff>
--- a/InputData/fuels/IMFPbFT/Intnl Market Fuel Price by Fuel Type.xlsx
+++ b/InputData/fuels/IMFPbFT/Intnl Market Fuel Price by Fuel Type.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\fuels\IMFPbFT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Virginia\Models\eps-virginia\InputData\fuels\IMFPbFT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="9795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="9795" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -560,19 +560,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="91.3984375" customWidth="1"/>
+    <col min="2" max="2" width="91.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,43 +580,43 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -633,17 +633,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.59765625" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>30</v>
       </c>
@@ -750,7 +750,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -857,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -964,7 +964,7 @@
         <v>2.0477634967012055E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>3.9079957744775265E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>2.0477634967012055E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1499,12 +1499,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>1.1906757518E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>4.2423075188889903E-6</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>1.2545426900000001E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>9.4849426860000013E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>5.245594982E-6</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>4.2423075188889903E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2360,12 +2360,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>6.5422931799999996E-7</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -3221,12 +3221,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -3333,7 +3333,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>2.2011E-6</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>6.9286799999999997E-6</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>3.2346599999999999E-6</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>2.65089E-6</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>2.2011E-6</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>29</v>
       </c>
@@ -4082,12 +4082,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>2.7944125074000001E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>27</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -4943,12 +4943,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -5162,7 +5162,7 @@
         <v>2.6648697335999999E-5</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>2.1893294264E-5</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>25</v>
       </c>
@@ -5376,7 +5376,7 @@
         <v>2.7079282736E-5</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>2.2930386300000003E-5</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>27</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>2.27495971E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>28</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>2.1893294264E-5</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -5804,12 +5804,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>30</v>
       </c>
@@ -5916,7 +5916,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>3.0938504238000002E-5</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>24</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>25</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -6344,7 +6344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>27</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>28</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>29</v>
       </c>
@@ -6665,12 +6665,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>30</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>23</v>
       </c>
@@ -6884,7 +6884,7 @@
         <v>2.7443025294669152E-5</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -6991,7 +6991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>25</v>
       </c>
@@ -7098,7 +7098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>27</v>
       </c>
@@ -7312,7 +7312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>29</v>
       </c>
@@ -7526,12 +7526,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>30</v>
       </c>
@@ -7638,7 +7638,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>23</v>
       </c>
@@ -7745,7 +7745,7 @@
         <v>2.0870261376000001E-5</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>24</v>
       </c>
@@ -7852,7 +7852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>25</v>
       </c>
@@ -7959,7 +7959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>27</v>
       </c>
@@ -8173,7 +8173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>28</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>29</v>
       </c>
@@ -8387,12 +8387,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>30</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>23</v>
       </c>
@@ -8606,7 +8606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -8713,7 +8713,7 @@
         <v>1.8783936654525313E-6</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>25</v>
       </c>
@@ -8820,7 +8820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -8927,7 +8927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>27</v>
       </c>
@@ -9034,7 +9034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>28</v>
       </c>
@@ -9141,7 +9141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>29</v>
       </c>
@@ -9248,12 +9248,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>30</v>
       </c>
@@ -9360,7 +9360,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>23</v>
       </c>
@@ -9467,7 +9467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -9574,7 +9574,7 @@
         <v>1.6704703340094422E-5</v>
       </c>
     </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>25</v>
       </c>
@@ -9681,7 +9681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>26</v>
       </c>
@@ -9788,7 +9788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>27</v>
       </c>
@@ -9895,7 +9895,7 @@
         <v>1.6704703340094422E-5</v>
       </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>28</v>
       </c>
@@ -10002,7 +10002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>29</v>
       </c>
@@ -10109,12 +10109,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>30</v>
       </c>
@@ -10221,7 +10221,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>23</v>
       </c>
@@ -10328,7 +10328,7 @@
         <v>1.5088604480000001E-5</v>
       </c>
     </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>24</v>
       </c>
@@ -10435,7 +10435,7 @@
         <v>1.5882854028E-5</v>
       </c>
     </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>25</v>
       </c>
@@ -10542,7 +10542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>26</v>
       </c>
@@ -10649,7 +10649,7 @@
         <v>1.356775875E-5</v>
       </c>
     </row>
-    <row r="106" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>27</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>1.5380589091999999E-5</v>
       </c>
     </row>
-    <row r="107" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>28</v>
       </c>
@@ -10863,7 +10863,7 @@
         <v>1.5380589091999999E-5</v>
       </c>
     </row>
-    <row r="108" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>29</v>
       </c>
@@ -10970,12 +10970,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="110" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>30</v>
       </c>
@@ -11082,7 +11082,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="111" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>23</v>
       </c>
@@ -11189,7 +11189,7 @@
         <v>2.0712846811999998E-5</v>
       </c>
     </row>
-    <row r="112" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>24</v>
       </c>
@@ -11296,7 +11296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>25</v>
       </c>
@@ -11403,7 +11403,7 @@
         <v>3.2981201010000001E-5</v>
       </c>
     </row>
-    <row r="114" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>26</v>
       </c>
@@ -11510,7 +11510,7 @@
         <v>2.2380442554E-5</v>
       </c>
     </row>
-    <row r="115" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>27</v>
       </c>
@@ -11617,7 +11617,7 @@
         <v>1.7201462633999998E-5</v>
       </c>
     </row>
-    <row r="116" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>28</v>
       </c>
@@ -11724,7 +11724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>29</v>
       </c>
@@ -11831,12 +11831,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="119" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>30</v>
       </c>
@@ -11943,7 +11943,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="120" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>23</v>
       </c>
@@ -12050,7 +12050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>24</v>
       </c>
@@ -12157,7 +12157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>25</v>
       </c>
@@ -12264,7 +12264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>26</v>
       </c>
@@ -12371,7 +12371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>27</v>
       </c>
@@ -12478,7 +12478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>28</v>
       </c>
@@ -12585,7 +12585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>29</v>
       </c>
@@ -12692,12 +12692,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>30</v>
       </c>
@@ -12804,7 +12804,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="129" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>23</v>
       </c>
@@ -12911,7 +12911,7 @@
         <v>2.8046695015698495E-5</v>
       </c>
     </row>
-    <row r="130" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>24</v>
       </c>
@@ -13018,7 +13018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>25</v>
       </c>
@@ -13125,7 +13125,7 @@
         <v>2.8046695015698495E-5</v>
       </c>
     </row>
-    <row r="132" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>26</v>
       </c>
@@ -13232,7 +13232,7 @@
         <v>2.8046695015698495E-5</v>
       </c>
     </row>
-    <row r="133" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>27</v>
       </c>
@@ -13339,7 +13339,7 @@
         <v>2.8046695015698495E-5</v>
       </c>
     </row>
-    <row r="134" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>28</v>
       </c>
@@ -13446,7 +13446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>29</v>
       </c>
@@ -13565,15 +13565,17 @@
   </sheetPr>
   <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.59765625" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -13680,7 +13682,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
@@ -13787,430 +13789,430 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6">
-        <f>MAX('Data from BFCpUEbS'!B3:B9)</f>
-        <v>3.3366807140683847E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B3:B9)</f>
+        <v>1.0252637187383837E-6</v>
       </c>
       <c r="C3" s="6">
-        <f>MAX('Data from BFCpUEbS'!C3:C9)</f>
-        <v>3.8828610656292297E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C3:C9)</f>
+        <v>1.106408393280366E-6</v>
       </c>
       <c r="D3" s="6">
-        <f>MAX('Data from BFCpUEbS'!D3:D9)</f>
-        <v>3.7700807200587562E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D3:D9)</f>
+        <v>1.0877181795587404E-6</v>
       </c>
       <c r="E3" s="6">
-        <f>MAX('Data from BFCpUEbS'!E3:E9)</f>
-        <v>3.7454719118854008E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E3:E9)</f>
+        <v>1.084107495673296E-6</v>
       </c>
       <c r="F3" s="6">
-        <f>MAX('Data from BFCpUEbS'!F3:F9)</f>
-        <v>3.6280074768803021E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F3:F9)</f>
+        <v>1.0916580296667233E-6</v>
       </c>
       <c r="G3" s="6">
-        <f>MAX('Data from BFCpUEbS'!G3:G9)</f>
-        <v>3.6010025309560283E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G3:G9)</f>
+        <v>1.0896018094564352E-6</v>
       </c>
       <c r="H3" s="6">
-        <f>MAX('Data from BFCpUEbS'!H3:H9)</f>
-        <v>3.5775782489518555E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H3:H9)</f>
+        <v>1.0866609417601667E-6</v>
       </c>
       <c r="I3" s="6">
-        <f>MAX('Data from BFCpUEbS'!I3:I9)</f>
-        <v>3.57650238165868E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I3:I9)</f>
+        <v>1.0768029806432762E-6</v>
       </c>
       <c r="J3" s="6">
-        <f>MAX('Data from BFCpUEbS'!J3:J9)</f>
-        <v>3.5966850736844447E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J3:J9)</f>
+        <v>1.0827700118949983E-6</v>
       </c>
       <c r="K3" s="6">
-        <f>MAX('Data from BFCpUEbS'!K3:K9)</f>
-        <v>3.617606824274601E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K3:K9)</f>
+        <v>1.0844984268238363E-6</v>
       </c>
       <c r="L3" s="6">
-        <f>MAX('Data from BFCpUEbS'!L3:L9)</f>
-        <v>3.6401557656063247E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L3:L9)</f>
+        <v>1.0891250483248809E-6</v>
       </c>
       <c r="M3" s="6">
-        <f>MAX('Data from BFCpUEbS'!M3:M9)</f>
-        <v>3.6531821312347782E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M3:M9)</f>
+        <v>1.0920909429693115E-6</v>
       </c>
       <c r="N3" s="6">
-        <f>MAX('Data from BFCpUEbS'!N3:N9)</f>
-        <v>3.6789454419927968E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N3:N9)</f>
+        <v>1.1018097830151604E-6</v>
       </c>
       <c r="O3" s="6">
-        <f>MAX('Data from BFCpUEbS'!O3:O9)</f>
-        <v>3.7026602442336667E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O3:O9)</f>
+        <v>1.1101178890541885E-6</v>
       </c>
       <c r="P3" s="6">
-        <f>MAX('Data from BFCpUEbS'!P3:P9)</f>
-        <v>3.7293161529833779E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P3:P9)</f>
+        <v>1.1127755486120372E-6</v>
       </c>
       <c r="Q3" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q3:Q9)</f>
-        <v>3.7458608594983294E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q3:Q9)</f>
+        <v>1.111858194433776E-6</v>
       </c>
       <c r="R3" s="6">
-        <f>MAX('Data from BFCpUEbS'!R3:R9)</f>
-        <v>3.7551362960753955E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R3:R9)</f>
+        <v>1.1138497600132441E-6</v>
       </c>
       <c r="S3" s="6">
-        <f>MAX('Data from BFCpUEbS'!S3:S9)</f>
-        <v>3.76767977941768E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S3:S9)</f>
+        <v>1.1149248610839022E-6</v>
       </c>
       <c r="T3" s="6">
-        <f>MAX('Data from BFCpUEbS'!T3:T9)</f>
-        <v>3.7709725136246255E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T3:T9)</f>
+        <v>1.1170959749795179E-6</v>
       </c>
       <c r="U3" s="6">
-        <f>MAX('Data from BFCpUEbS'!U3:U9)</f>
-        <v>3.7871609068460637E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U3:U9)</f>
+        <v>1.1211258377538508E-6</v>
       </c>
       <c r="V3" s="6">
-        <f>MAX('Data from BFCpUEbS'!V3:V9)</f>
-        <v>3.7988628155304854E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V3:V9)</f>
+        <v>1.1242238506248326E-6</v>
       </c>
       <c r="W3" s="6">
-        <f>MAX('Data from BFCpUEbS'!W3:W9)</f>
-        <v>3.810728331358171E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W3:W9)</f>
+        <v>1.1274031585597558E-6</v>
       </c>
       <c r="X3" s="6">
-        <f>MAX('Data from BFCpUEbS'!X3:X9)</f>
-        <v>3.8184063580696542E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X3:X9)</f>
+        <v>1.130044273124938E-6</v>
       </c>
       <c r="Y3" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y3:Y9)</f>
-        <v>3.8221363006023168E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y3:Y9)</f>
+        <v>1.1315104362286418E-6</v>
       </c>
       <c r="Z3" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z3:Z9)</f>
-        <v>3.8304174662192471E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z3:Z9)</f>
+        <v>1.1328777114641193E-6</v>
       </c>
       <c r="AA3" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA3:AA9)</f>
-        <v>3.8379894143046001E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA3:AA9)</f>
+        <v>1.1338543189281321E-6</v>
       </c>
       <c r="AB3" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB3:AB9)</f>
-        <v>3.8441244588575927E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB3:AB9)</f>
+        <v>1.134223341273984E-6</v>
       </c>
       <c r="AC3" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC3:AC9)</f>
-        <v>3.8532554033323572E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC3:AC9)</f>
+        <v>1.135161093414364E-6</v>
       </c>
       <c r="AD3" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD3:AD9)</f>
-        <v>3.8693192675865772E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD3:AD9)</f>
+        <v>1.1376973190759471E-6</v>
       </c>
       <c r="AE3" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE3:AE9)</f>
-        <v>3.87568620803071E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE3:AE9)</f>
+        <v>1.1387447430618745E-6</v>
       </c>
       <c r="AF3" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF3:AF9)</f>
-        <v>3.8841184433989304E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF3:AF9)</f>
+        <v>1.1392917560746852E-6</v>
       </c>
       <c r="AG3" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG3:AG9)</f>
-        <v>3.8925808909711001E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG3:AG9)</f>
+        <v>1.1407163799259531E-6</v>
       </c>
       <c r="AH3" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH3:AH9)</f>
-        <v>3.9003409270086809E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH3:AH9)</f>
+        <v>1.1422309389936383E-6</v>
       </c>
       <c r="AI3" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI3:AI9)</f>
-        <v>3.9079957744775265E-6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI3:AI9)</f>
+        <v>1.1433603954114197E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="6">
-        <f>MAX('Data from BFCpUEbS'!B12:B18)</f>
-        <v>1.3476261865999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B12:B18)</f>
+        <v>5.7376995022857146E-6</v>
       </c>
       <c r="C4" s="6">
-        <f>MAX('Data from BFCpUEbS'!C12:C18)</f>
-        <v>1.3154913176E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C12:C18)</f>
+        <v>5.6690840859999997E-6</v>
       </c>
       <c r="D4" s="6">
-        <f>MAX('Data from BFCpUEbS'!D12:D18)</f>
-        <v>1.2909810365999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D12:D18)</f>
+        <v>5.490156573428571E-6</v>
       </c>
       <c r="E4" s="6">
-        <f>MAX('Data from BFCpUEbS'!E12:E18)</f>
-        <v>1.2796294308000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E12:E18)</f>
+        <v>5.5251503691428579E-6</v>
       </c>
       <c r="F4" s="6">
-        <f>MAX('Data from BFCpUEbS'!F12:F18)</f>
-        <v>1.2072592764E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F12:F18)</f>
+        <v>5.4222715349037986E-6</v>
       </c>
       <c r="G4" s="6">
-        <f>MAX('Data from BFCpUEbS'!G12:G18)</f>
-        <v>1.213775091E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G12:G18)</f>
+        <v>5.4879388237810596E-6</v>
       </c>
       <c r="H4" s="6">
-        <f>MAX('Data from BFCpUEbS'!H12:H18)</f>
-        <v>1.2132397612000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H12:H18)</f>
+        <v>5.6053540999457218E-6</v>
       </c>
       <c r="I4" s="6">
-        <f>MAX('Data from BFCpUEbS'!I12:I18)</f>
-        <v>1.2140205914E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I12:I18)</f>
+        <v>5.7424679994493232E-6</v>
       </c>
       <c r="J4" s="6">
-        <f>MAX('Data from BFCpUEbS'!J12:J18)</f>
-        <v>1.2215556988000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J12:J18)</f>
+        <v>5.8856484543616465E-6</v>
       </c>
       <c r="K4" s="6">
-        <f>MAX('Data from BFCpUEbS'!K12:K18)</f>
-        <v>1.2101059294000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K12:K18)</f>
+        <v>5.9199151530267739E-6</v>
       </c>
       <c r="L4" s="6">
-        <f>MAX('Data from BFCpUEbS'!L12:L18)</f>
-        <v>1.1890639128E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L12:L18)</f>
+        <v>5.905927022843132E-6</v>
       </c>
       <c r="M4" s="6">
-        <f>MAX('Data from BFCpUEbS'!M12:M18)</f>
-        <v>1.1750807182000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M12:M18)</f>
+        <v>5.9311436715810243E-6</v>
       </c>
       <c r="N4" s="6">
-        <f>MAX('Data from BFCpUEbS'!N12:N18)</f>
-        <v>1.2165593178E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N12:N18)</f>
+        <v>6.0650223055374571E-6</v>
       </c>
       <c r="O4" s="6">
-        <f>MAX('Data from BFCpUEbS'!O12:O18)</f>
-        <v>1.1984095627999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O12:O18)</f>
+        <v>6.0634337807409586E-6</v>
       </c>
       <c r="P4" s="6">
-        <f>MAX('Data from BFCpUEbS'!P12:P18)</f>
-        <v>1.1896743734E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P12:P18)</f>
+        <v>6.0616773323869495E-6</v>
       </c>
       <c r="Q4" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q12:Q18)</f>
-        <v>1.186323101E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q12:Q18)</f>
+        <v>6.1328666772211428E-6</v>
       </c>
       <c r="R4" s="6">
-        <f>MAX('Data from BFCpUEbS'!R12:R18)</f>
-        <v>1.1793633565999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R12:R18)</f>
+        <v>6.167334351299095E-6</v>
       </c>
       <c r="S4" s="6">
-        <f>MAX('Data from BFCpUEbS'!S12:S18)</f>
-        <v>1.1726569730000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S12:S18)</f>
+        <v>6.1864583843504292E-6</v>
       </c>
       <c r="T4" s="6">
-        <f>MAX('Data from BFCpUEbS'!T12:T18)</f>
-        <v>1.1672418886000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T12:T18)</f>
+        <v>6.2059808949822803E-6</v>
       </c>
       <c r="U4" s="6">
-        <f>MAX('Data from BFCpUEbS'!U12:U18)</f>
-        <v>1.1645428465999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U12:U18)</f>
+        <v>6.243570988297672E-6</v>
       </c>
       <c r="V4" s="6">
-        <f>MAX('Data from BFCpUEbS'!V12:V18)</f>
-        <v>1.1654211092E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V12:V18)</f>
+        <v>6.2601476393664876E-6</v>
       </c>
       <c r="W4" s="6">
-        <f>MAX('Data from BFCpUEbS'!W12:W18)</f>
-        <v>1.1682280032E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W12:W18)</f>
+        <v>6.2569907505741453E-6</v>
       </c>
       <c r="X4" s="6">
-        <f>MAX('Data from BFCpUEbS'!X12:X18)</f>
-        <v>1.1723742728000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X12:X18)</f>
+        <v>6.2671619489103117E-6</v>
       </c>
       <c r="Y4" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y12:Y18)</f>
-        <v>1.178227803E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y12:Y18)</f>
+        <v>6.3047220263125154E-6</v>
       </c>
       <c r="Z4" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z12:Z18)</f>
-        <v>1.1817871017999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z12:Z18)</f>
+        <v>6.3004777048611255E-6</v>
       </c>
       <c r="AA4" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA12:AA18)</f>
-        <v>1.1872902044E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA12:AA18)</f>
+        <v>6.3292327391125154E-6</v>
       </c>
       <c r="AB4" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB12:AB18)</f>
-        <v>1.1943786400000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB12:AB18)</f>
+        <v>6.3715149930756514E-6</v>
       </c>
       <c r="AC4" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC12:AC18)</f>
-        <v>1.2011399549999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC12:AC18)</f>
+        <v>6.4262742231749995E-6</v>
       </c>
       <c r="AD4" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD12:AD18)</f>
-        <v>1.2097864863999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD12:AD18)</f>
+        <v>6.4823172822711534E-6</v>
       </c>
       <c r="AE4" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE12:AE18)</f>
-        <v>1.2171380626E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE12:AE18)</f>
+        <v>6.5268454412102716E-6</v>
       </c>
       <c r="AF4" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF12:AF18)</f>
-        <v>1.2248336683999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF12:AF18)</f>
+        <v>6.5810913370959009E-6</v>
       </c>
       <c r="AG4" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG12:AG18)</f>
-        <v>1.2344197918E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG12:AG18)</f>
+        <v>6.6695949032078427E-6</v>
       </c>
       <c r="AH4" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH12:AH18)</f>
-        <v>1.2462597478000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH12:AH18)</f>
+        <v>6.747900422245257E-6</v>
       </c>
       <c r="AI4" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI12:AI18)</f>
-        <v>1.2545426900000001E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI12:AI18)</f>
+        <v>6.8096195891111398E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="6">
-        <f>MAX('Data from BFCpUEbS'!B21:B27)</f>
-        <v>6.0297219800000004E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B21:B27)</f>
+        <v>8.6138885428571428E-8</v>
       </c>
       <c r="C5" s="6">
-        <f>MAX('Data from BFCpUEbS'!C21:C27)</f>
-        <v>6.0483584400000002E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C21:C27)</f>
+        <v>8.640512057142858E-8</v>
       </c>
       <c r="D5" s="6">
-        <f>MAX('Data from BFCpUEbS'!D21:D27)</f>
-        <v>6.0576812399999998E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D21:D27)</f>
+        <v>8.6538303428571425E-8</v>
       </c>
       <c r="E5" s="6">
-        <f>MAX('Data from BFCpUEbS'!E21:E27)</f>
-        <v>6.0763177000000006E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E21:E27)</f>
+        <v>8.6804538571428577E-8</v>
       </c>
       <c r="F5" s="6">
-        <f>MAX('Data from BFCpUEbS'!F21:F27)</f>
-        <v>6.0856405000000002E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F21:F27)</f>
+        <v>8.6937721428571435E-8</v>
       </c>
       <c r="G5" s="6">
-        <f>MAX('Data from BFCpUEbS'!G21:G27)</f>
-        <v>6.0949541599999994E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G21:G27)</f>
+        <v>8.7070773714285702E-8</v>
       </c>
       <c r="H5" s="6">
-        <f>MAX('Data from BFCpUEbS'!H21:H27)</f>
-        <v>6.1135997600000006E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H21:H27)</f>
+        <v>8.7337139428571432E-8</v>
       </c>
       <c r="I5" s="6">
-        <f>MAX('Data from BFCpUEbS'!I21:I27)</f>
-        <v>6.1229134199999998E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I21:I27)</f>
+        <v>8.7470191714285712E-8</v>
       </c>
       <c r="J5" s="6">
-        <f>MAX('Data from BFCpUEbS'!J21:J27)</f>
-        <v>6.1415498800000007E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J21:J27)</f>
+        <v>8.7736426857142864E-8</v>
       </c>
       <c r="K5" s="6">
-        <f>MAX('Data from BFCpUEbS'!K21:K27)</f>
-        <v>6.1508726800000003E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K21:K27)</f>
+        <v>8.7869609714285722E-8</v>
       </c>
       <c r="L5" s="6">
-        <f>MAX('Data from BFCpUEbS'!L21:L27)</f>
-        <v>6.1601954799999998E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L21:L27)</f>
+        <v>8.8002792571428567E-8</v>
       </c>
       <c r="M5" s="6">
-        <f>MAX('Data from BFCpUEbS'!M21:M27)</f>
-        <v>6.169509139999999E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M21:M27)</f>
+        <v>8.8135844857142847E-8</v>
       </c>
       <c r="N5" s="6">
-        <f>MAX('Data from BFCpUEbS'!N21:N27)</f>
-        <v>6.1881547400000002E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N21:N27)</f>
+        <v>8.8402210571428577E-8</v>
       </c>
       <c r="O5" s="6">
-        <f>MAX('Data from BFCpUEbS'!O21:O27)</f>
-        <v>6.2067912000000011E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O21:O27)</f>
+        <v>8.8668445714285729E-8</v>
       </c>
       <c r="P5" s="6">
-        <f>MAX('Data from BFCpUEbS'!P21:P27)</f>
-        <v>6.2161140000000007E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P21:P27)</f>
+        <v>8.8801628571428587E-8</v>
       </c>
       <c r="Q5" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q21:Q27)</f>
-        <v>6.2347504600000005E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q21:Q27)</f>
+        <v>8.9067863714285725E-8</v>
       </c>
       <c r="R5" s="6">
-        <f>MAX('Data from BFCpUEbS'!R21:R27)</f>
-        <v>6.2533869200000003E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R21:R27)</f>
+        <v>8.9334098857142864E-8</v>
       </c>
       <c r="S5" s="6">
-        <f>MAX('Data from BFCpUEbS'!S21:S27)</f>
-        <v>6.2627097199999999E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S21:S27)</f>
+        <v>8.9467281714285709E-8</v>
       </c>
       <c r="T5" s="6">
-        <f>MAX('Data from BFCpUEbS'!T21:T27)</f>
-        <v>6.2813461800000008E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T21:T27)</f>
+        <v>8.9733516857142874E-8</v>
       </c>
       <c r="U5" s="6">
-        <f>MAX('Data from BFCpUEbS'!U21:U27)</f>
-        <v>6.2999826400000006E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U21:U27)</f>
+        <v>8.9999752000000012E-8</v>
       </c>
       <c r="V5" s="6">
-        <f>MAX('Data from BFCpUEbS'!V21:V27)</f>
-        <v>6.3093054400000001E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V21:V27)</f>
+        <v>9.0132934857142857E-8</v>
       </c>
       <c r="W5" s="6">
-        <f>MAX('Data from BFCpUEbS'!W21:W27)</f>
-        <v>6.327941900000001E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W21:W27)</f>
+        <v>9.0399170000000009E-8</v>
       </c>
       <c r="X5" s="6">
-        <f>MAX('Data from BFCpUEbS'!X21:X27)</f>
-        <v>6.3465783599999998E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X21:X27)</f>
+        <v>9.0665405142857134E-8</v>
       </c>
       <c r="Y5" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y21:Y27)</f>
-        <v>6.3652239599999999E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y21:Y27)</f>
+        <v>9.0931770857142851E-8</v>
       </c>
       <c r="Z5" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z21:Z27)</f>
-        <v>6.3745376200000002E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z21:Z27)</f>
+        <v>9.1064823142857144E-8</v>
       </c>
       <c r="AA5" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA21:AA27)</f>
-        <v>6.3931832200000004E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA21:AA27)</f>
+        <v>9.1331188857142861E-8</v>
       </c>
       <c r="AB5" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB21:AB27)</f>
-        <v>6.4118196800000002E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB21:AB27)</f>
+        <v>9.1597423999999999E-8</v>
       </c>
       <c r="AC5" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC21:AC27)</f>
-        <v>6.4304561400000011E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC21:AC27)</f>
+        <v>9.1863659142857164E-8</v>
       </c>
       <c r="AD5" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD21:AD27)</f>
-        <v>6.4490925999999998E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD21:AD27)</f>
+        <v>9.2129894285714289E-8</v>
       </c>
       <c r="AE5" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE21:AE27)</f>
-        <v>6.4677382E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE21:AE27)</f>
+        <v>9.2396260000000006E-8</v>
       </c>
       <c r="AF5" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF21:AF27)</f>
-        <v>6.4863746599999998E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF21:AF27)</f>
+        <v>9.2662495142857144E-8</v>
       </c>
       <c r="AG5" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG21:AG27)</f>
-        <v>6.5050111200000007E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG21:AG27)</f>
+        <v>9.2928730285714296E-8</v>
       </c>
       <c r="AH5" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH21:AH27)</f>
-        <v>6.5236567200000009E-7</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH21:AH27)</f>
+        <v>9.3195096000000012E-8</v>
       </c>
       <c r="AI5" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI21:AI27)</f>
-        <v>6.5422931799999996E-7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI21:AI27)</f>
+        <v>9.3461331142857138E-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -14317,7 +14319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -14424,7 +14426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -14531,853 +14533,853 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="6">
-        <f>MAX('Data from BFCpUEbS'!B30:B36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B30:B36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="C9" s="6">
-        <f>MAX('Data from BFCpUEbS'!C30:C36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C30:C36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="D9" s="6">
-        <f>MAX('Data from BFCpUEbS'!D30:D36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D30:D36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="E9" s="6">
-        <f>MAX('Data from BFCpUEbS'!E30:E36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E30:E36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="F9" s="6">
-        <f>MAX('Data from BFCpUEbS'!F30:F36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F30:F36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="G9" s="6">
-        <f>MAX('Data from BFCpUEbS'!G30:G36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G30:G36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="H9" s="6">
-        <f>MAX('Data from BFCpUEbS'!H30:H36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H30:H36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="I9" s="6">
-        <f>MAX('Data from BFCpUEbS'!I30:I36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I30:I36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="J9" s="6">
-        <f>MAX('Data from BFCpUEbS'!J30:J36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J30:J36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="K9" s="6">
-        <f>MAX('Data from BFCpUEbS'!K30:K36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K30:K36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="L9" s="6">
-        <f>MAX('Data from BFCpUEbS'!L30:L36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L30:L36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="M9" s="6">
-        <f>MAX('Data from BFCpUEbS'!M30:M36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M30:M36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="N9" s="6">
-        <f>MAX('Data from BFCpUEbS'!N30:N36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N30:N36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="O9" s="6">
-        <f>MAX('Data from BFCpUEbS'!O30:O36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O30:O36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="P9" s="6">
-        <f>MAX('Data from BFCpUEbS'!P30:P36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P30:P36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="Q9" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q30:Q36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q30:Q36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="R9" s="6">
-        <f>MAX('Data from BFCpUEbS'!R30:R36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R30:R36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="S9" s="6">
-        <f>MAX('Data from BFCpUEbS'!S30:S36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S30:S36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="T9" s="6">
-        <f>MAX('Data from BFCpUEbS'!T30:T36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T30:T36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="U9" s="6">
-        <f>MAX('Data from BFCpUEbS'!U30:U36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U30:U36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="V9" s="6">
-        <f>MAX('Data from BFCpUEbS'!V30:V36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V30:V36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="W9" s="6">
-        <f>MAX('Data from BFCpUEbS'!W30:W36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W30:W36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="X9" s="6">
-        <f>MAX('Data from BFCpUEbS'!X30:X36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X30:X36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="Y9" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y30:Y36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y30:Y36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="Z9" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z30:Z36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z30:Z36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="AA9" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA30:AA36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA30:AA36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="AB9" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB30:AB36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB30:AB36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="AC9" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC30:AC36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC30:AC36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="AD9" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD30:AD36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD30:AD36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="AE9" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE30:AE36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE30:AE36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="AF9" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF30:AF36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF30:AF36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="AG9" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG30:AG36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG30:AG36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="AH9" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH30:AH36)</f>
-        <v>6.9286799999999997E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH30:AH36)</f>
+        <v>2.4594900000000005E-6</v>
       </c>
       <c r="AI9" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI30:AI36)</f>
-        <v>6.9286799999999997E-6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI30:AI36)</f>
+        <v>2.4594900000000005E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="6">
-        <f>MAX('Data from BFCpUEbS'!B39:B45)</f>
-        <v>1.9669752538000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B39:B45)</f>
+        <v>2.8099646482857147E-6</v>
       </c>
       <c r="C10" s="6">
-        <f>MAX('Data from BFCpUEbS'!C39:C45)</f>
-        <v>2.19950901E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C39:C45)</f>
+        <v>3.1421557285714284E-6</v>
       </c>
       <c r="D10" s="6">
-        <f>MAX('Data from BFCpUEbS'!D39:D45)</f>
-        <v>2.2150654727999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D39:D45)</f>
+        <v>3.1643792468571427E-6</v>
       </c>
       <c r="E10" s="6">
-        <f>MAX('Data from BFCpUEbS'!E39:E45)</f>
-        <v>2.2814232438000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E39:E45)</f>
+        <v>3.259176062571429E-6</v>
       </c>
       <c r="F10" s="6">
-        <f>MAX('Data from BFCpUEbS'!F39:F45)</f>
-        <v>2.2984676072000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F39:F45)</f>
+        <v>3.2835251531428573E-6</v>
       </c>
       <c r="G10" s="6">
-        <f>MAX('Data from BFCpUEbS'!G39:G45)</f>
-        <v>2.3046926784E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G39:G45)</f>
+        <v>3.2924181120000001E-6</v>
       </c>
       <c r="H10" s="6">
-        <f>MAX('Data from BFCpUEbS'!H39:H45)</f>
-        <v>2.3366409086000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H39:H45)</f>
+        <v>3.338058440857143E-6</v>
       </c>
       <c r="I10" s="6">
-        <f>MAX('Data from BFCpUEbS'!I39:I45)</f>
-        <v>2.3687142654000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I39:I45)</f>
+        <v>3.3838775219999999E-6</v>
       </c>
       <c r="J10" s="6">
-        <f>MAX('Data from BFCpUEbS'!J39:J45)</f>
-        <v>2.3952283086000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J39:J45)</f>
+        <v>3.4217547265714286E-6</v>
       </c>
       <c r="K10" s="6">
-        <f>MAX('Data from BFCpUEbS'!K39:K45)</f>
-        <v>2.4149314980000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K39:K45)</f>
+        <v>3.4499021399999999E-6</v>
       </c>
       <c r="L10" s="6">
-        <f>MAX('Data from BFCpUEbS'!L39:L45)</f>
-        <v>2.4648281290000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L39:L45)</f>
+        <v>3.5211830414285716E-6</v>
       </c>
       <c r="M10" s="6">
-        <f>MAX('Data from BFCpUEbS'!M39:M45)</f>
-        <v>2.4824144030000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M39:M45)</f>
+        <v>3.5463062900000004E-6</v>
       </c>
       <c r="N10" s="6">
-        <f>MAX('Data from BFCpUEbS'!N39:N45)</f>
-        <v>2.5432679746E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N39:N45)</f>
+        <v>3.6332399637142855E-6</v>
       </c>
       <c r="O10" s="6">
-        <f>MAX('Data from BFCpUEbS'!O39:O45)</f>
-        <v>2.5537889371999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O39:O45)</f>
+        <v>3.6482699102857141E-6</v>
       </c>
       <c r="P10" s="6">
-        <f>MAX('Data from BFCpUEbS'!P39:P45)</f>
-        <v>2.5815483054000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P39:P45)</f>
+        <v>3.6879261505714288E-6</v>
       </c>
       <c r="Q10" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q39:Q45)</f>
-        <v>2.6032051697999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q39:Q45)</f>
+        <v>3.7188645282857141E-6</v>
       </c>
       <c r="R10" s="6">
-        <f>MAX('Data from BFCpUEbS'!R39:R45)</f>
-        <v>2.6137934942E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R39:R45)</f>
+        <v>3.7339907060000001E-6</v>
       </c>
       <c r="S10" s="6">
-        <f>MAX('Data from BFCpUEbS'!S39:S45)</f>
-        <v>2.6328497544000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S39:S45)</f>
+        <v>3.7612139348571432E-6</v>
       </c>
       <c r="T10" s="6">
-        <f>MAX('Data from BFCpUEbS'!T39:T45)</f>
-        <v>2.6497424852000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T39:T45)</f>
+        <v>3.7853464074285719E-6</v>
       </c>
       <c r="U10" s="6">
-        <f>MAX('Data from BFCpUEbS'!U39:U45)</f>
-        <v>2.6717591914000004E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U39:U45)</f>
+        <v>3.8167988448571432E-6</v>
       </c>
       <c r="V10" s="6">
-        <f>MAX('Data from BFCpUEbS'!V39:V45)</f>
-        <v>2.6715942144000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V39:V45)</f>
+        <v>3.8165631634285719E-6</v>
       </c>
       <c r="W10" s="6">
-        <f>MAX('Data from BFCpUEbS'!W39:W45)</f>
-        <v>2.6869800334E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W39:W45)</f>
+        <v>3.8385429048571427E-6</v>
       </c>
       <c r="X10" s="6">
-        <f>MAX('Data from BFCpUEbS'!X39:X45)</f>
-        <v>2.7041538192000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X39:X45)</f>
+        <v>3.8630768845714287E-6</v>
       </c>
       <c r="Y10" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y39:Y45)</f>
-        <v>2.7231755301999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y39:Y45)</f>
+        <v>3.8902507574285714E-6</v>
       </c>
       <c r="Z10" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z39:Z45)</f>
-        <v>2.7326333280000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z39:Z45)</f>
+        <v>3.9037618971428571E-6</v>
       </c>
       <c r="AA10" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA39:AA45)</f>
-        <v>2.7541183604000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA39:AA45)</f>
+        <v>3.9344548005714285E-6</v>
       </c>
       <c r="AB10" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB39:AB45)</f>
-        <v>2.7584776834000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB39:AB45)</f>
+        <v>3.9406824048571435E-6</v>
       </c>
       <c r="AC10" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC39:AC45)</f>
-        <v>2.7585664328000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC39:AC45)</f>
+        <v>3.9408091897142857E-6</v>
       </c>
       <c r="AD10" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD39:AD45)</f>
-        <v>2.7646289034000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD39:AD45)</f>
+        <v>3.9494698620000002E-6</v>
       </c>
       <c r="AE10" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE39:AE45)</f>
-        <v>2.7732988332000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE39:AE45)</f>
+        <v>3.961855476E-6</v>
       </c>
       <c r="AF10" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF39:AF45)</f>
-        <v>2.7802421255999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF39:AF45)</f>
+        <v>3.971774465142857E-6</v>
       </c>
       <c r="AG10" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG39:AG45)</f>
-        <v>2.7936297578E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG39:AG45)</f>
+        <v>3.990899654E-6</v>
       </c>
       <c r="AH10" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH39:AH45)</f>
-        <v>2.7951322824000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH39:AH45)</f>
+        <v>3.993046117714286E-6</v>
       </c>
       <c r="AI10" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI39:AI45)</f>
-        <v>2.7944125074000001E-5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI39:AI45)</f>
+        <v>3.9920178677142857E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="6">
-        <f>MAX('Data from BFCpUEbS'!B48:B54)</f>
-        <v>1.7901774918000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B48:B54)</f>
+        <v>1.4727069951999999E-5</v>
       </c>
       <c r="C11" s="6">
-        <f>MAX('Data from BFCpUEbS'!C48:C54)</f>
-        <v>2.1168004188000005E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C48:C54)</f>
+        <v>1.7539630621428574E-5</v>
       </c>
       <c r="D11" s="6">
-        <f>MAX('Data from BFCpUEbS'!D48:D54)</f>
-        <v>2.0770838284000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D48:D54)</f>
+        <v>1.7753879663999999E-5</v>
       </c>
       <c r="E11" s="6">
-        <f>MAX('Data from BFCpUEbS'!E48:E54)</f>
-        <v>2.2119300872000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E48:E54)</f>
+        <v>1.7775267525142859E-5</v>
       </c>
       <c r="F11" s="6">
-        <f>MAX('Data from BFCpUEbS'!F48:F54)</f>
-        <v>2.2191779244E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F48:F54)</f>
+        <v>1.7450298872857145E-5</v>
       </c>
       <c r="G11" s="6">
-        <f>MAX('Data from BFCpUEbS'!G48:G54)</f>
-        <v>2.2003592127999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G48:G54)</f>
+        <v>1.6992545867428576E-5</v>
       </c>
       <c r="H11" s="6">
-        <f>MAX('Data from BFCpUEbS'!H48:H54)</f>
-        <v>2.2243018997999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H48:H54)</f>
+        <v>1.6862599614857141E-5</v>
       </c>
       <c r="I11" s="6">
-        <f>MAX('Data from BFCpUEbS'!I48:I54)</f>
-        <v>2.3027634985999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I48:I54)</f>
+        <v>1.7023925707142857E-5</v>
       </c>
       <c r="J11" s="6">
-        <f>MAX('Data from BFCpUEbS'!J48:J54)</f>
-        <v>2.3508396244000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J48:J54)</f>
+        <v>1.7376708032285712E-5</v>
       </c>
       <c r="K11" s="6">
-        <f>MAX('Data from BFCpUEbS'!K48:K54)</f>
-        <v>2.3893345624000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K48:K54)</f>
+        <v>1.766827808E-5</v>
       </c>
       <c r="L11" s="6">
-        <f>MAX('Data from BFCpUEbS'!L48:L54)</f>
-        <v>2.4530954766000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L48:L54)</f>
+        <v>1.8193104975428574E-5</v>
       </c>
       <c r="M11" s="6">
-        <f>MAX('Data from BFCpUEbS'!M48:M54)</f>
-        <v>2.4709093366E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M48:M54)</f>
+        <v>1.8327606604000001E-5</v>
       </c>
       <c r="N11" s="6">
-        <f>MAX('Data from BFCpUEbS'!N48:N54)</f>
-        <v>2.5138533523999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N48:N54)</f>
+        <v>1.8798500318E-5</v>
       </c>
       <c r="O11" s="6">
-        <f>MAX('Data from BFCpUEbS'!O48:O54)</f>
-        <v>2.5324812208E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O48:O54)</f>
+        <v>1.8933153931714285E-5</v>
       </c>
       <c r="P11" s="6">
-        <f>MAX('Data from BFCpUEbS'!P48:P54)</f>
-        <v>2.5529170726E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P48:P54)</f>
+        <v>1.9082934245428572E-5</v>
       </c>
       <c r="Q11" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q48:Q54)</f>
-        <v>2.5807853895999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q48:Q54)</f>
+        <v>1.9314895432857143E-5</v>
       </c>
       <c r="R11" s="6">
-        <f>MAX('Data from BFCpUEbS'!R48:R54)</f>
-        <v>2.6107867998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R48:R54)</f>
+        <v>1.9554559812285713E-5</v>
       </c>
       <c r="S11" s="6">
-        <f>MAX('Data from BFCpUEbS'!S48:S54)</f>
-        <v>2.6174430048000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S48:S54)</f>
+        <v>1.9606921174857146E-5</v>
       </c>
       <c r="T11" s="6">
-        <f>MAX('Data from BFCpUEbS'!T48:T54)</f>
-        <v>2.6386481703999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T48:T54)</f>
+        <v>1.979452254742857E-5</v>
       </c>
       <c r="U11" s="6">
-        <f>MAX('Data from BFCpUEbS'!U48:U54)</f>
-        <v>2.6725586672000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U48:U54)</f>
+        <v>2.0074990106571432E-5</v>
       </c>
       <c r="V11" s="6">
-        <f>MAX('Data from BFCpUEbS'!V48:V54)</f>
-        <v>2.6640547198000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V48:V54)</f>
+        <v>2.0018733928857145E-5</v>
       </c>
       <c r="W11" s="6">
-        <f>MAX('Data from BFCpUEbS'!W48:W54)</f>
-        <v>2.6796499362000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W48:W54)</f>
+        <v>2.0138501094000003E-5</v>
       </c>
       <c r="X11" s="6">
-        <f>MAX('Data from BFCpUEbS'!X48:X54)</f>
-        <v>2.6940904964E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X48:X54)</f>
+        <v>2.0266726154E-5</v>
       </c>
       <c r="Y11" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y48:Y54)</f>
-        <v>2.7105847232000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y48:Y54)</f>
+        <v>2.0394291567142857E-5</v>
       </c>
       <c r="Z11" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z48:Z54)</f>
-        <v>2.7143374244000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z48:Z54)</f>
+        <v>2.0435181446285717E-5</v>
       </c>
       <c r="AA11" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA48:AA54)</f>
-        <v>2.7303142357999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA48:AA54)</f>
+        <v>2.0587988666857144E-5</v>
       </c>
       <c r="AB11" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB48:AB54)</f>
-        <v>2.7314966776000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB48:AB54)</f>
+        <v>2.0603174124000001E-5</v>
       </c>
       <c r="AC11" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC48:AC54)</f>
-        <v>2.7245307180000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC48:AC54)</f>
+        <v>2.054674128314286E-5</v>
       </c>
       <c r="AD11" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD48:AD54)</f>
-        <v>2.7300943274000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD48:AD54)</f>
+        <v>2.0589944626857146E-5</v>
       </c>
       <c r="AE11" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE48:AE54)</f>
-        <v>2.7209806506000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE48:AE54)</f>
+        <v>2.0536102062000003E-5</v>
       </c>
       <c r="AF11" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF48:AF54)</f>
-        <v>2.7122061592000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF48:AF54)</f>
+        <v>2.0483475508857147E-5</v>
       </c>
       <c r="AG11" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG48:AG54)</f>
-        <v>2.7161640534000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG48:AG54)</f>
+        <v>2.0522300400857145E-5</v>
       </c>
       <c r="AH11" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH48:AH54)</f>
-        <v>2.7103823636E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH48:AH54)</f>
+        <v>2.0474307044285719E-5</v>
       </c>
       <c r="AI11" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI48:AI54)</f>
-        <v>2.7079282736E-5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI48:AI54)</f>
+        <v>2.045636457142857E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="6">
-        <f>MAX('Data from BFCpUEbS'!B57:B63)</f>
-        <v>2.024200154E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B57:B63)</f>
+        <v>2.8917145057142857E-6</v>
       </c>
       <c r="C12" s="6">
-        <f>MAX('Data from BFCpUEbS'!C57:C63)</f>
-        <v>2.6718902590000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C57:C63)</f>
+        <v>3.8169860842857143E-6</v>
       </c>
       <c r="D12" s="6">
-        <f>MAX('Data from BFCpUEbS'!D57:D63)</f>
-        <v>3.1123721768000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D57:D63)</f>
+        <v>4.4462459668571431E-6</v>
       </c>
       <c r="E12" s="6">
-        <f>MAX('Data from BFCpUEbS'!E57:E63)</f>
-        <v>3.0155874372000004E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E57:E63)</f>
+        <v>4.3079820531428573E-6</v>
       </c>
       <c r="F12" s="6">
-        <f>MAX('Data from BFCpUEbS'!F57:F63)</f>
-        <v>2.9887357624000004E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F57:F63)</f>
+        <v>4.2696225177142859E-6</v>
       </c>
       <c r="G12" s="6">
-        <f>MAX('Data from BFCpUEbS'!G57:G63)</f>
-        <v>2.9039987310000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G57:G63)</f>
+        <v>4.1485696157142859E-6</v>
       </c>
       <c r="H12" s="6">
-        <f>MAX('Data from BFCpUEbS'!H57:H63)</f>
-        <v>2.8808476593999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H57:H63)</f>
+        <v>4.1154966562857139E-6</v>
       </c>
       <c r="I12" s="6">
-        <f>MAX('Data from BFCpUEbS'!I57:I63)</f>
-        <v>2.6872917988E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I57:I63)</f>
+        <v>3.8389882840000003E-6</v>
       </c>
       <c r="J12" s="6">
-        <f>MAX('Data from BFCpUEbS'!J57:J63)</f>
-        <v>2.4666933287999997E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J57:J63)</f>
+        <v>3.5238476125714283E-6</v>
       </c>
       <c r="K12" s="6">
-        <f>MAX('Data from BFCpUEbS'!K57:K63)</f>
-        <v>2.4502367588E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K57:K63)</f>
+        <v>3.5003382268571429E-6</v>
       </c>
       <c r="L12" s="6">
-        <f>MAX('Data from BFCpUEbS'!L57:L63)</f>
-        <v>2.3940137853999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L57:L63)</f>
+        <v>3.4200196934285712E-6</v>
       </c>
       <c r="M12" s="6">
-        <f>MAX('Data from BFCpUEbS'!M57:M63)</f>
-        <v>2.3291538776000005E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M57:M63)</f>
+        <v>3.3273626822857149E-6</v>
       </c>
       <c r="N12" s="6">
-        <f>MAX('Data from BFCpUEbS'!N57:N63)</f>
-        <v>2.3532325678000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N57:N63)</f>
+        <v>3.3617608111428572E-6</v>
       </c>
       <c r="O12" s="6">
-        <f>MAX('Data from BFCpUEbS'!O57:O63)</f>
-        <v>2.2664109766000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O57:O63)</f>
+        <v>3.2377299665714288E-6</v>
       </c>
       <c r="P12" s="6">
-        <f>MAX('Data from BFCpUEbS'!P57:P63)</f>
-        <v>2.2721157076000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P57:P63)</f>
+        <v>3.2458795822857143E-6</v>
       </c>
       <c r="Q12" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q57:Q63)</f>
-        <v>2.2771843860000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q57:Q63)</f>
+        <v>3.2531205514285715E-6</v>
       </c>
       <c r="R12" s="6">
-        <f>MAX('Data from BFCpUEbS'!R57:R63)</f>
-        <v>2.2544802604000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R57:R63)</f>
+        <v>3.2206860862857144E-6</v>
       </c>
       <c r="S12" s="6">
-        <f>MAX('Data from BFCpUEbS'!S57:S63)</f>
-        <v>2.2233066452000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S57:S63)</f>
+        <v>3.1761523502857147E-6</v>
       </c>
       <c r="T12" s="6">
-        <f>MAX('Data from BFCpUEbS'!T57:T63)</f>
-        <v>2.2239800804000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T57:T63)</f>
+        <v>3.1771144005714285E-6</v>
       </c>
       <c r="U12" s="6">
-        <f>MAX('Data from BFCpUEbS'!U57:U63)</f>
-        <v>2.2269196871999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U57:U63)</f>
+        <v>3.1813138388571427E-6</v>
       </c>
       <c r="V12" s="6">
-        <f>MAX('Data from BFCpUEbS'!V57:V63)</f>
-        <v>2.2140268032000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V57:V63)</f>
+        <v>3.1628954331428573E-6</v>
       </c>
       <c r="W12" s="6">
-        <f>MAX('Data from BFCpUEbS'!W57:W63)</f>
-        <v>2.2329942226000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W57:W63)</f>
+        <v>3.1899917465714286E-6</v>
       </c>
       <c r="X12" s="6">
-        <f>MAX('Data from BFCpUEbS'!X57:X63)</f>
-        <v>2.271043677E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X57:X63)</f>
+        <v>3.2443481100000002E-6</v>
       </c>
       <c r="Y12" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y57:Y63)</f>
-        <v>2.3162615420000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y57:Y63)</f>
+        <v>3.3089450600000002E-6</v>
       </c>
       <c r="Z12" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z57:Z63)</f>
-        <v>2.3817468999999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z57:Z63)</f>
+        <v>3.4024955714285713E-6</v>
       </c>
       <c r="AA12" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA57:AA63)</f>
-        <v>2.4558087769999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA57:AA63)</f>
+        <v>3.5082982528571427E-6</v>
       </c>
       <c r="AB12" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB57:AB63)</f>
-        <v>2.5342010032E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB57:AB63)</f>
+        <v>3.6202871474285715E-6</v>
       </c>
       <c r="AC12" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC57:AC63)</f>
-        <v>2.5831278802000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC57:AC63)</f>
+        <v>3.6901826860000003E-6</v>
       </c>
       <c r="AD12" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD57:AD63)</f>
-        <v>2.6324827834E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD57:AD63)</f>
+        <v>3.7606896905714287E-6</v>
       </c>
       <c r="AE12" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE57:AE63)</f>
-        <v>2.7745894011999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE57:AE63)</f>
+        <v>3.963699144571428E-6</v>
       </c>
       <c r="AF12" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF57:AF63)</f>
-        <v>2.9673261350000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF57:AF63)</f>
+        <v>4.2390373357142859E-6</v>
       </c>
       <c r="AG12" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG57:AG63)</f>
-        <v>3.1078583878000009E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG57:AG63)</f>
+        <v>4.4397976968571443E-6</v>
       </c>
       <c r="AH12" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH57:AH63)</f>
-        <v>3.1048696078E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH57:AH63)</f>
+        <v>4.4355280111428574E-6</v>
       </c>
       <c r="AI12" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI57:AI63)</f>
-        <v>3.0938504238000002E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI57:AI63)</f>
+        <v>4.4197863197142856E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="6">
-        <f>MAX('Data from BFCpUEbS'!B66:B72)</f>
-        <v>1.8435380000000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B66:B72)</f>
+        <v>2.6336257142857143E-6</v>
       </c>
       <c r="C13" s="6">
-        <f>MAX('Data from BFCpUEbS'!C66:C72)</f>
-        <v>2.1798967020582415E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C66:C72)</f>
+        <v>3.114138145797488E-6</v>
       </c>
       <c r="D13" s="6">
-        <f>MAX('Data from BFCpUEbS'!D66:D72)</f>
-        <v>2.1385085113765126E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D66:D72)</f>
+        <v>3.0550121591093038E-6</v>
       </c>
       <c r="E13" s="6">
-        <f>MAX('Data from BFCpUEbS'!E66:E72)</f>
-        <v>2.2778619370285807E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E66:E72)</f>
+        <v>3.254088481469401E-6</v>
       </c>
       <c r="F13" s="6">
-        <f>MAX('Data from BFCpUEbS'!F66:F72)</f>
-        <v>2.2853258132962789E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F66:F72)</f>
+        <v>3.264751161851827E-6</v>
       </c>
       <c r="G13" s="6">
-        <f>MAX('Data from BFCpUEbS'!G66:G72)</f>
-        <v>2.2659461651303547E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G66:G72)</f>
+        <v>3.2370659501862209E-6</v>
       </c>
       <c r="H13" s="6">
-        <f>MAX('Data from BFCpUEbS'!H66:H72)</f>
-        <v>2.2906025209994171E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H66:H72)</f>
+        <v>3.2722893157134532E-6</v>
       </c>
       <c r="I13" s="6">
-        <f>MAX('Data from BFCpUEbS'!I66:I72)</f>
-        <v>2.3375943134078121E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I66:I72)</f>
+        <v>3.3394204477254459E-6</v>
       </c>
       <c r="J13" s="6">
-        <f>MAX('Data from BFCpUEbS'!J66:J72)</f>
-        <v>2.3739446841006885E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J66:J72)</f>
+        <v>3.3913495487152691E-6</v>
       </c>
       <c r="K13" s="6">
-        <f>MAX('Data from BFCpUEbS'!K66:K72)</f>
-        <v>2.3909990832147169E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K66:K72)</f>
+        <v>3.415712976021024E-6</v>
       </c>
       <c r="L13" s="6">
-        <f>MAX('Data from BFCpUEbS'!L66:L72)</f>
-        <v>2.4566336239012736E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L66:L72)</f>
+        <v>3.5094766055732479E-6</v>
       </c>
       <c r="M13" s="6">
-        <f>MAX('Data from BFCpUEbS'!M66:M72)</f>
-        <v>2.4784958029829904E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M66:M72)</f>
+        <v>3.5407082899757008E-6</v>
       </c>
       <c r="N13" s="6">
-        <f>MAX('Data from BFCpUEbS'!N66:N72)</f>
-        <v>2.5574207082310615E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N66:N72)</f>
+        <v>3.6534581546158021E-6</v>
       </c>
       <c r="O13" s="6">
-        <f>MAX('Data from BFCpUEbS'!O66:O72)</f>
-        <v>2.577319358310528E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O66:O72)</f>
+        <v>3.6818847975864687E-6</v>
       </c>
       <c r="P13" s="6">
-        <f>MAX('Data from BFCpUEbS'!P66:P72)</f>
-        <v>2.6050968791148584E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P66:P72)</f>
+        <v>3.7215669701640833E-6</v>
       </c>
       <c r="Q13" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q66:Q72)</f>
-        <v>2.6348784024112508E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q66:Q72)</f>
+        <v>3.7641120034446441E-6</v>
       </c>
       <c r="R13" s="6">
-        <f>MAX('Data from BFCpUEbS'!R66:R72)</f>
-        <v>2.6608846903521348E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R66:R72)</f>
+        <v>3.8012638433601925E-6</v>
       </c>
       <c r="S13" s="6">
-        <f>MAX('Data from BFCpUEbS'!S66:S72)</f>
-        <v>2.6694894484105561E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S66:S72)</f>
+        <v>3.8135563548722229E-6</v>
       </c>
       <c r="T13" s="6">
-        <f>MAX('Data from BFCpUEbS'!T66:T72)</f>
-        <v>2.695014195947073E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T66:T72)</f>
+        <v>3.8500202799243899E-6</v>
       </c>
       <c r="U13" s="6">
-        <f>MAX('Data from BFCpUEbS'!U66:U72)</f>
-        <v>2.7262039143157375E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U66:U72)</f>
+        <v>3.8945770204510535E-6</v>
       </c>
       <c r="V13" s="6">
-        <f>MAX('Data from BFCpUEbS'!V66:V72)</f>
-        <v>2.7203371407808988E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V66:V72)</f>
+        <v>3.8861959154012843E-6</v>
       </c>
       <c r="W13" s="6">
-        <f>MAX('Data from BFCpUEbS'!W66:W72)</f>
-        <v>2.7371973612682245E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W66:W72)</f>
+        <v>3.910281944668892E-6</v>
       </c>
       <c r="X13" s="6">
-        <f>MAX('Data from BFCpUEbS'!X66:X72)</f>
-        <v>2.7521051594319003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X66:X72)</f>
+        <v>3.9315787991884289E-6</v>
       </c>
       <c r="Y13" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y66:Y72)</f>
-        <v>2.765077007041034E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y66:Y72)</f>
+        <v>3.95011001005862E-6</v>
       </c>
       <c r="Z13" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z66:Z72)</f>
-        <v>2.7671349428113807E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z66:Z72)</f>
+        <v>3.9530499183019725E-6</v>
       </c>
       <c r="AA13" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA66:AA72)</f>
-        <v>2.7829163094842299E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA66:AA72)</f>
+        <v>3.9755947278346143E-6</v>
       </c>
       <c r="AB13" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB66:AB72)</f>
-        <v>2.7829572535960167E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB66:AB72)</f>
+        <v>3.9756532194228809E-6</v>
       </c>
       <c r="AC13" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC66:AC72)</f>
-        <v>2.7715345994027325E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC66:AC72)</f>
+        <v>3.9593351420039033E-6</v>
       </c>
       <c r="AD13" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD66:AD72)</f>
-        <v>2.775472387588253E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD66:AD72)</f>
+        <v>3.9649605536975042E-6</v>
       </c>
       <c r="AE13" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE66:AE72)</f>
-        <v>2.7624993163619855E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE66:AE72)</f>
+        <v>3.9464275948028364E-6</v>
       </c>
       <c r="AF13" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF66:AF72)</f>
-        <v>2.7486248158056496E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF66:AF72)</f>
+        <v>3.9266068797223564E-6</v>
       </c>
       <c r="AG13" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG66:AG72)</f>
-        <v>2.7510461658647501E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG66:AG72)</f>
+        <v>3.9300659512353571E-6</v>
       </c>
       <c r="AH13" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH66:AH72)</f>
-        <v>2.7452752109639312E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH66:AH72)</f>
+        <v>3.9218217299484734E-6</v>
       </c>
       <c r="AI13" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI66:AI72)</f>
-        <v>2.7443025294669152E-5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI66:AI72)</f>
+        <v>3.9204321849527364E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="6">
-        <f>MAX('Data from BFCpUEbS'!B75:B81)</f>
-        <v>1.1299246395999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B75:B81)</f>
+        <v>1.6141780565714285E-6</v>
       </c>
       <c r="C14" s="6">
-        <f>MAX('Data from BFCpUEbS'!C75:C81)</f>
-        <v>1.4766924008000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C75:C81)</f>
+        <v>2.1095605725714286E-6</v>
       </c>
       <c r="D14" s="6">
-        <f>MAX('Data from BFCpUEbS'!D75:D81)</f>
-        <v>1.4826091797999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D75:D81)</f>
+        <v>2.1180131139999998E-6</v>
       </c>
       <c r="E14" s="6">
-        <f>MAX('Data from BFCpUEbS'!E75:E81)</f>
-        <v>1.5895791698000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E75:E81)</f>
+        <v>2.2708273854285716E-6</v>
       </c>
       <c r="F14" s="6">
-        <f>MAX('Data from BFCpUEbS'!F75:F81)</f>
-        <v>1.5719448194E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F75:F81)</f>
+        <v>2.2456354562857144E-6</v>
       </c>
       <c r="G14" s="6">
-        <f>MAX('Data from BFCpUEbS'!G75:G81)</f>
-        <v>1.5506510871999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G75:G81)</f>
+        <v>2.2152158388571423E-6</v>
       </c>
       <c r="H14" s="6">
-        <f>MAX('Data from BFCpUEbS'!H75:H81)</f>
-        <v>1.5739347802000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H75:H81)</f>
+        <v>2.2484782574285719E-6</v>
       </c>
       <c r="I14" s="6">
-        <f>MAX('Data from BFCpUEbS'!I75:I81)</f>
-        <v>1.5995871956000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I75:I81)</f>
+        <v>2.2851245651428576E-6</v>
       </c>
       <c r="J14" s="6">
-        <f>MAX('Data from BFCpUEbS'!J75:J81)</f>
-        <v>1.6253077040000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J75:J81)</f>
+        <v>2.321868148571429E-6</v>
       </c>
       <c r="K14" s="6">
-        <f>MAX('Data from BFCpUEbS'!K75:K81)</f>
-        <v>1.6604643484000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K75:K81)</f>
+        <v>2.3720919262857142E-6</v>
       </c>
       <c r="L14" s="6">
-        <f>MAX('Data from BFCpUEbS'!L75:L81)</f>
-        <v>1.7064871732000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L75:L81)</f>
+        <v>2.4378388188571433E-6</v>
       </c>
       <c r="M14" s="6">
-        <f>MAX('Data from BFCpUEbS'!M75:M81)</f>
-        <v>1.7414155918E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M75:M81)</f>
+        <v>2.4877365597142856E-6</v>
       </c>
       <c r="N14" s="6">
-        <f>MAX('Data from BFCpUEbS'!N75:N81)</f>
-        <v>1.8059955413999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N75:N81)</f>
+        <v>2.5799936305714282E-6</v>
       </c>
       <c r="O14" s="6">
-        <f>MAX('Data from BFCpUEbS'!O75:O81)</f>
-        <v>1.8171074050000004E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O75:O81)</f>
+        <v>2.5958677214285721E-6</v>
       </c>
       <c r="P14" s="6">
-        <f>MAX('Data from BFCpUEbS'!P75:P81)</f>
-        <v>1.8412333490000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P75:P81)</f>
+        <v>2.630333355714286E-6</v>
       </c>
       <c r="Q14" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q75:Q81)</f>
-        <v>1.8778595226000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q75:Q81)</f>
+        <v>2.6826564608571429E-6</v>
       </c>
       <c r="R14" s="6">
-        <f>MAX('Data from BFCpUEbS'!R75:R81)</f>
-        <v>1.898228104E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R75:R81)</f>
+        <v>2.7117544342857145E-6</v>
       </c>
       <c r="S14" s="6">
-        <f>MAX('Data from BFCpUEbS'!S75:S81)</f>
-        <v>1.9127841024E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S75:S81)</f>
+        <v>2.7325487177142856E-6</v>
       </c>
       <c r="T14" s="6">
-        <f>MAX('Data from BFCpUEbS'!T75:T81)</f>
-        <v>1.9382394594000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T75:T81)</f>
+        <v>2.7689135134285716E-6</v>
       </c>
       <c r="U14" s="6">
-        <f>MAX('Data from BFCpUEbS'!U75:U81)</f>
-        <v>1.9684162661999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U75:U81)</f>
+        <v>2.8120232374285714E-6</v>
       </c>
       <c r="V14" s="6">
-        <f>MAX('Data from BFCpUEbS'!V75:V81)</f>
-        <v>1.9723126482000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V75:V81)</f>
+        <v>2.8175894974285714E-6</v>
       </c>
       <c r="W14" s="6">
-        <f>MAX('Data from BFCpUEbS'!W75:W81)</f>
-        <v>1.9911092410000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W75:W81)</f>
+        <v>2.8444417728571429E-6</v>
       </c>
       <c r="X14" s="6">
-        <f>MAX('Data from BFCpUEbS'!X75:X81)</f>
-        <v>2.0085458932000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X75:X81)</f>
+        <v>2.8693512760000003E-6</v>
       </c>
       <c r="Y14" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y75:Y81)</f>
-        <v>2.0194853764000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y75:Y81)</f>
+        <v>2.8849791091428574E-6</v>
       </c>
       <c r="Z14" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z75:Z81)</f>
-        <v>2.0300547809999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z75:Z81)</f>
+        <v>2.9000782585714284E-6</v>
       </c>
       <c r="AA14" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA75:AA81)</f>
-        <v>2.0515664108E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA75:AA81)</f>
+        <v>2.9308091582857143E-6</v>
       </c>
       <c r="AB14" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB75:AB81)</f>
-        <v>2.0616605354000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB75:AB81)</f>
+        <v>2.9452293362857143E-6</v>
       </c>
       <c r="AC14" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC75:AC81)</f>
-        <v>2.0582075347999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC75:AC81)</f>
+        <v>2.9402964782857141E-6</v>
       </c>
       <c r="AD14" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD75:AD81)</f>
-        <v>2.0732332378000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD75:AD81)</f>
+        <v>2.9617617682857144E-6</v>
       </c>
       <c r="AE14" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE75:AE81)</f>
-        <v>2.0721237332E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE75:AE81)</f>
+        <v>2.9601767617142859E-6</v>
       </c>
       <c r="AF14" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF75:AF81)</f>
-        <v>2.0776910900000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF75:AF81)</f>
+        <v>2.9681301285714288E-6</v>
       </c>
       <c r="AG14" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG75:AG81)</f>
-        <v>2.0909362296000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG75:AG81)</f>
+        <v>2.9870517565714288E-6</v>
       </c>
       <c r="AH14" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH75:AH81)</f>
-        <v>2.0877794564E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH75:AH81)</f>
+        <v>2.9825420805714288E-6</v>
       </c>
       <c r="AI14" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI75:AI81)</f>
-        <v>2.0870261376000001E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI75:AI81)</f>
+        <v>2.9814659108571431E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -15484,7 +15486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -15591,887 +15593,887 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="6">
-        <f>MAX('Data from BFCpUEbS'!B84:B90)</f>
-        <v>1.7612732665544324E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B84:B90)</f>
+        <v>2.5161046665063318E-7</v>
       </c>
       <c r="C17" s="6">
-        <f>MAX('Data from BFCpUEbS'!C84:C90)</f>
-        <v>1.7712865776652133E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C84:C90)</f>
+        <v>2.5304093966645904E-7</v>
       </c>
       <c r="D17" s="6">
-        <f>MAX('Data from BFCpUEbS'!D84:D90)</f>
-        <v>1.7630075047224427E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D84:D90)</f>
+        <v>2.5185821496034898E-7</v>
       </c>
       <c r="E17" s="6">
-        <f>MAX('Data from BFCpUEbS'!E84:E90)</f>
-        <v>1.7627020566608279E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E84:E90)</f>
+        <v>2.5181457952297542E-7</v>
       </c>
       <c r="F17" s="6">
-        <f>MAX('Data from BFCpUEbS'!F84:F90)</f>
-        <v>1.8408176636909316E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F84:F90)</f>
+        <v>2.6297395195584737E-7</v>
       </c>
       <c r="G17" s="6">
-        <f>MAX('Data from BFCpUEbS'!G84:G90)</f>
-        <v>1.8466018234031597E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G84:G90)</f>
+        <v>2.6380026048616569E-7</v>
       </c>
       <c r="H17" s="6">
-        <f>MAX('Data from BFCpUEbS'!H84:H90)</f>
-        <v>1.8479035538475611E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H84:H90)</f>
+        <v>2.6398622197822302E-7</v>
       </c>
       <c r="I17" s="6">
-        <f>MAX('Data from BFCpUEbS'!I84:I90)</f>
-        <v>1.8167478515628743E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I84:I90)</f>
+        <v>2.5953540736612488E-7</v>
       </c>
       <c r="J17" s="6">
-        <f>MAX('Data from BFCpUEbS'!J84:J90)</f>
-        <v>1.8266484077418191E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J84:J90)</f>
+        <v>2.6094977253454559E-7</v>
       </c>
       <c r="K17" s="6">
-        <f>MAX('Data from BFCpUEbS'!K84:K90)</f>
-        <v>1.8226018520164622E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K84:K90)</f>
+        <v>2.6037169314520887E-7</v>
       </c>
       <c r="L17" s="6">
-        <f>MAX('Data from BFCpUEbS'!L84:L90)</f>
-        <v>1.8271137321993203E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L84:L90)</f>
+        <v>2.6101624745704578E-7</v>
       </c>
       <c r="M17" s="6">
-        <f>MAX('Data from BFCpUEbS'!M84:M90)</f>
-        <v>1.8306613052785682E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M84:M90)</f>
+        <v>2.6152304361122401E-7</v>
       </c>
       <c r="N17" s="6">
-        <f>MAX('Data from BFCpUEbS'!N84:N90)</f>
-        <v>1.8500475804618694E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N84:N90)</f>
+        <v>2.6429251149455278E-7</v>
       </c>
       <c r="O17" s="6">
-        <f>MAX('Data from BFCpUEbS'!O84:O90)</f>
-        <v>1.8658442098301625E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O84:O90)</f>
+        <v>2.6654917283288038E-7</v>
       </c>
       <c r="P17" s="6">
-        <f>MAX('Data from BFCpUEbS'!P84:P90)</f>
-        <v>1.8621510650851861E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P84:P90)</f>
+        <v>2.6602158072645517E-7</v>
       </c>
       <c r="Q17" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q84:Q90)</f>
-        <v>1.8516177349604167E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q84:Q90)</f>
+        <v>2.6451681928005952E-7</v>
       </c>
       <c r="R17" s="6">
-        <f>MAX('Data from BFCpUEbS'!R84:R90)</f>
-        <v>1.8537575543011493E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R84:R90)</f>
+        <v>2.6482250775730706E-7</v>
       </c>
       <c r="S17" s="6">
-        <f>MAX('Data from BFCpUEbS'!S84:S90)</f>
-        <v>1.8514561756551003E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S84:S90)</f>
+        <v>2.6449373937930005E-7</v>
       </c>
       <c r="T17" s="6">
-        <f>MAX('Data from BFCpUEbS'!T84:T90)</f>
-        <v>1.8569163753019789E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T84:T90)</f>
+        <v>2.6527376790028268E-7</v>
       </c>
       <c r="U17" s="6">
-        <f>MAX('Data from BFCpUEbS'!U84:U90)</f>
-        <v>1.8624295865959145E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U84:U90)</f>
+        <v>2.6606136951370206E-7</v>
       </c>
       <c r="V17" s="6">
-        <f>MAX('Data from BFCpUEbS'!V84:V90)</f>
-        <v>1.8670087831559878E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V84:V90)</f>
+        <v>2.6671554045085538E-7</v>
       </c>
       <c r="W17" s="6">
-        <f>MAX('Data from BFCpUEbS'!W84:W90)</f>
-        <v>1.8717739412081184E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W84:W90)</f>
+        <v>2.6739627731544547E-7</v>
       </c>
       <c r="X17" s="6">
-        <f>MAX('Data from BFCpUEbS'!X84:X90)</f>
-        <v>1.8767317923900276E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X84:X90)</f>
+        <v>2.6810454177000396E-7</v>
       </c>
       <c r="Y17" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y84:Y90)</f>
-        <v>1.8797282126308253E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y84:Y90)</f>
+        <v>2.6853260180440363E-7</v>
       </c>
       <c r="Z17" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z84:Z90)</f>
-        <v>1.880319755295605E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z84:Z90)</f>
+        <v>2.6861710789937214E-7</v>
       </c>
       <c r="AA17" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA84:AA90)</f>
-        <v>1.8799823319548132E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA84:AA90)</f>
+        <v>2.6856890456497333E-7</v>
       </c>
       <c r="AB17" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB84:AB90)</f>
-        <v>1.878353275626202E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB84:AB90)</f>
+        <v>2.6833618223231456E-7</v>
       </c>
       <c r="AC17" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC84:AC90)</f>
-        <v>1.8771760804796488E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC84:AC90)</f>
+        <v>2.681680114970927E-7</v>
       </c>
       <c r="AD17" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD84:AD90)</f>
-        <v>1.8779510602723406E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD84:AD90)</f>
+        <v>2.6827872289604867E-7</v>
       </c>
       <c r="AE17" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE84:AE90)</f>
-        <v>1.8783936654525313E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE84:AE90)</f>
+        <v>2.6834195220750446E-7</v>
       </c>
       <c r="AF17" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF84:AF90)</f>
-        <v>1.8762824555721152E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF84:AF90)</f>
+        <v>2.6804035079601648E-7</v>
       </c>
       <c r="AG17" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG84:AG90)</f>
-        <v>1.8769749728027177E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG84:AG90)</f>
+        <v>2.6813928182895965E-7</v>
       </c>
       <c r="AH17" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH84:AH90)</f>
-        <v>1.8782783861565499E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH84:AH90)</f>
+        <v>2.6832548373664999E-7</v>
       </c>
       <c r="AI17" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI84:AI90)</f>
-        <v>1.8783936654525313E-6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI84:AI90)</f>
+        <v>2.6834195220750446E-7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
       <c r="B18" s="6">
-        <f>MAX('Data from BFCpUEbS'!B93:B99)</f>
-        <v>8.2769078342367539E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B93:B99)</f>
+        <v>2.3648308097819296E-6</v>
       </c>
       <c r="C18" s="6">
-        <f>MAX('Data from BFCpUEbS'!C93:C99)</f>
-        <v>1.0941789343941251E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C93:C99)</f>
+        <v>3.1262255268403574E-6</v>
       </c>
       <c r="D18" s="6">
-        <f>MAX('Data from BFCpUEbS'!D93:D99)</f>
-        <v>1.0849100570379438E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D93:D99)</f>
+        <v>3.0997430201084108E-6</v>
       </c>
       <c r="E18" s="6">
-        <f>MAX('Data from BFCpUEbS'!E93:E99)</f>
-        <v>1.1142998317188317E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E93:E99)</f>
+        <v>3.1837138049109477E-6</v>
       </c>
       <c r="F18" s="6">
-        <f>MAX('Data from BFCpUEbS'!F93:F99)</f>
-        <v>1.1384257079559366E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F93:F99)</f>
+        <v>3.2526448798741048E-6</v>
       </c>
       <c r="G18" s="6">
-        <f>MAX('Data from BFCpUEbS'!G93:G99)</f>
-        <v>1.1270036486098968E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G93:G99)</f>
+        <v>3.220010424599705E-6</v>
       </c>
       <c r="H18" s="6">
-        <f>MAX('Data from BFCpUEbS'!H93:H99)</f>
-        <v>1.1522639620213325E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H93:H99)</f>
+        <v>3.2921827486323784E-6</v>
       </c>
       <c r="I18" s="6">
-        <f>MAX('Data from BFCpUEbS'!I93:I99)</f>
-        <v>1.2019459590837558E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I93:I99)</f>
+        <v>3.4341313116678737E-6</v>
       </c>
       <c r="J18" s="6">
-        <f>MAX('Data from BFCpUEbS'!J93:J99)</f>
-        <v>1.2452300840006993E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J93:J99)</f>
+        <v>3.5578002400019978E-6</v>
       </c>
       <c r="K18" s="6">
-        <f>MAX('Data from BFCpUEbS'!K93:K99)</f>
-        <v>1.2791358401468788E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K93:K99)</f>
+        <v>3.6546738289910822E-6</v>
       </c>
       <c r="L18" s="6">
-        <f>MAX('Data from BFCpUEbS'!L93:L99)</f>
-        <v>1.3159089416681239E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L93:L99)</f>
+        <v>3.7597398333374966E-6</v>
       </c>
       <c r="M18" s="6">
-        <f>MAX('Data from BFCpUEbS'!M93:M99)</f>
-        <v>1.3433050168910647E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M93:M99)</f>
+        <v>3.8380143339744705E-6</v>
       </c>
       <c r="N18" s="6">
-        <f>MAX('Data from BFCpUEbS'!N93:N99)</f>
-        <v>1.3737898495541178E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N93:N99)</f>
+        <v>3.9251138558689083E-6</v>
       </c>
       <c r="O18" s="6">
-        <f>MAX('Data from BFCpUEbS'!O93:O99)</f>
-        <v>1.3959282432593109E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O93:O99)</f>
+        <v>3.9883664093123165E-6</v>
       </c>
       <c r="P18" s="6">
-        <f>MAX('Data from BFCpUEbS'!P93:P99)</f>
-        <v>1.4257344081482776E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P93:P99)</f>
+        <v>4.0735268804236505E-6</v>
       </c>
       <c r="Q18" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q93:Q99)</f>
-        <v>1.4438483251267705E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q93:Q99)</f>
+        <v>4.1252809289336298E-6</v>
       </c>
       <c r="R18" s="6">
-        <f>MAX('Data from BFCpUEbS'!R93:R99)</f>
-        <v>1.486842252246896E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R93:R99)</f>
+        <v>4.2481207207054173E-6</v>
       </c>
       <c r="S18" s="6">
-        <f>MAX('Data from BFCpUEbS'!S93:S99)</f>
-        <v>1.4967983316663753E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S93:S99)</f>
+        <v>4.2765666619039298E-6</v>
       </c>
       <c r="T18" s="6">
-        <f>MAX('Data from BFCpUEbS'!T93:T99)</f>
-        <v>1.521432893093198E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T93:T99)</f>
+        <v>4.3469511231234228E-6</v>
       </c>
       <c r="U18" s="6">
-        <f>MAX('Data from BFCpUEbS'!U93:U99)</f>
-        <v>1.5521125760447631E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U93:U99)</f>
+        <v>4.4346073601278947E-6</v>
       </c>
       <c r="V18" s="6">
-        <f>MAX('Data from BFCpUEbS'!V93:V99)</f>
-        <v>1.5468901344290961E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V93:V99)</f>
+        <v>4.419686098368846E-6</v>
       </c>
       <c r="W18" s="6">
-        <f>MAX('Data from BFCpUEbS'!W93:W99)</f>
-        <v>1.5658013521944396E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W93:W99)</f>
+        <v>4.4737181491269699E-6</v>
       </c>
       <c r="X18" s="6">
-        <f>MAX('Data from BFCpUEbS'!X93:X99)</f>
-        <v>1.5778985473334501E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X93:X99)</f>
+        <v>4.5082815638098573E-6</v>
       </c>
       <c r="Y18" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y93:Y99)</f>
-        <v>1.6011257820947717E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y93:Y99)</f>
+        <v>4.5746450916993472E-6</v>
       </c>
       <c r="Z18" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z93:Z99)</f>
-        <v>1.6107150948417553E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z93:Z99)</f>
+        <v>4.6020431281193011E-6</v>
       </c>
       <c r="AA18" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA93:AA99)</f>
-        <v>1.6324436668648365E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA93:AA99)</f>
+        <v>4.6641247624709611E-6</v>
       </c>
       <c r="AB18" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB93:AB99)</f>
-        <v>1.6369952398321383E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB93:AB99)</f>
+        <v>4.6771292566632521E-6</v>
       </c>
       <c r="AC18" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC93:AC99)</f>
-        <v>1.6458011399895087E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC93:AC99)</f>
+        <v>4.7022889713985965E-6</v>
       </c>
       <c r="AD18" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD93:AD99)</f>
-        <v>1.6546032684385381E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD93:AD99)</f>
+        <v>4.7274379098243943E-6</v>
       </c>
       <c r="AE18" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE93:AE99)</f>
-        <v>1.6603596465116278E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE93:AE99)</f>
+        <v>4.7438847043189367E-6</v>
       </c>
       <c r="AF18" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF93:AF99)</f>
-        <v>1.6652577691554467E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF93:AF99)</f>
+        <v>4.7578793404441331E-6</v>
       </c>
       <c r="AG18" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG93:AG99)</f>
-        <v>1.6700591858366847E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG93:AG99)</f>
+        <v>4.7715976738190992E-6</v>
       </c>
       <c r="AH18" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH93:AH99)</f>
-        <v>1.6710367135513205E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH93:AH99)</f>
+        <v>4.7743906101466299E-6</v>
       </c>
       <c r="AI18" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI93:AI99)</f>
-        <v>1.6704703340094422E-5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI93:AI99)</f>
+        <v>4.7727723828841205E-6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="6">
-        <f>MAX('Data from BFCpUEbS'!B102:B108)</f>
-        <v>9.8917092459999995E-6</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B102:B108)</f>
+        <v>5.2511323857142856E-6</v>
       </c>
       <c r="C19" s="6">
-        <f>MAX('Data from BFCpUEbS'!C102:C108)</f>
-        <v>1.1619630816000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C102:C108)</f>
+        <v>6.5236825731428573E-6</v>
       </c>
       <c r="D19" s="6">
-        <f>MAX('Data from BFCpUEbS'!D102:D108)</f>
-        <v>1.1152867468000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D102:D108)</f>
+        <v>5.852465128857144E-6</v>
       </c>
       <c r="E19" s="6">
-        <f>MAX('Data from BFCpUEbS'!E102:E108)</f>
-        <v>1.1063360362000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E102:E108)</f>
+        <v>6.3348501731428569E-6</v>
       </c>
       <c r="F19" s="6">
-        <f>MAX('Data from BFCpUEbS'!F102:F108)</f>
-        <v>1.2787541844E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F102:F108)</f>
+        <v>6.9560792599999999E-6</v>
       </c>
       <c r="G19" s="6">
-        <f>MAX('Data from BFCpUEbS'!G102:G108)</f>
-        <v>1.2641682068E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G102:G108)</f>
+        <v>7.0613857699999997E-6</v>
       </c>
       <c r="H19" s="6">
-        <f>MAX('Data from BFCpUEbS'!H102:H108)</f>
-        <v>1.2817902182000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H102:H108)</f>
+        <v>7.5715130645714298E-6</v>
       </c>
       <c r="I19" s="6">
-        <f>MAX('Data from BFCpUEbS'!I102:I108)</f>
-        <v>1.3178264962000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I102:I108)</f>
+        <v>8.1965804291428585E-6</v>
       </c>
       <c r="J19" s="6">
-        <f>MAX('Data from BFCpUEbS'!J102:J108)</f>
-        <v>1.3455961926000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J102:J108)</f>
+        <v>8.368539736285715E-6</v>
       </c>
       <c r="K19" s="6">
-        <f>MAX('Data from BFCpUEbS'!K102:K108)</f>
-        <v>1.383774978E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K102:K108)</f>
+        <v>8.6214213391428569E-6</v>
       </c>
       <c r="L19" s="6">
-        <f>MAX('Data from BFCpUEbS'!L102:L108)</f>
-        <v>1.4332666156E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L102:L108)</f>
+        <v>8.9608080802857156E-6</v>
       </c>
       <c r="M19" s="6">
-        <f>MAX('Data from BFCpUEbS'!M102:M108)</f>
-        <v>1.4538236638000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M102:M108)</f>
+        <v>9.0834463805714299E-6</v>
       </c>
       <c r="N19" s="6">
-        <f>MAX('Data from BFCpUEbS'!N102:N108)</f>
-        <v>1.4894489160000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N102:N108)</f>
+        <v>9.3324710340000006E-6</v>
       </c>
       <c r="O19" s="6">
-        <f>MAX('Data from BFCpUEbS'!O102:O108)</f>
-        <v>1.4978873296E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O102:O108)</f>
+        <v>9.4589504845714287E-6</v>
       </c>
       <c r="P19" s="6">
-        <f>MAX('Data from BFCpUEbS'!P102:P108)</f>
-        <v>1.5147568448E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P102:P108)</f>
+        <v>9.5804563388571421E-6</v>
       </c>
       <c r="Q19" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q102:Q108)</f>
-        <v>1.5349951812E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q102:Q108)</f>
+        <v>9.7171503922857139E-6</v>
       </c>
       <c r="R19" s="6">
-        <f>MAX('Data from BFCpUEbS'!R102:R108)</f>
-        <v>1.5492804528E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R102:R108)</f>
+        <v>9.806601613714286E-6</v>
       </c>
       <c r="S19" s="6">
-        <f>MAX('Data from BFCpUEbS'!S102:S108)</f>
-        <v>1.5582407604000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S102:S108)</f>
+        <v>9.9499911088571439E-6</v>
       </c>
       <c r="T19" s="6">
-        <f>MAX('Data from BFCpUEbS'!T102:T108)</f>
-        <v>1.5732803562000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T102:T108)</f>
+        <v>1.0072632412285715E-5</v>
       </c>
       <c r="U19" s="6">
-        <f>MAX('Data from BFCpUEbS'!U102:U108)</f>
-        <v>1.5957438256000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U102:U108)</f>
+        <v>1.0222839564E-5</v>
       </c>
       <c r="V19" s="6">
-        <f>MAX('Data from BFCpUEbS'!V102:V108)</f>
-        <v>1.6018932176000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V102:V108)</f>
+        <v>1.0331572398857143E-5</v>
       </c>
       <c r="W19" s="6">
-        <f>MAX('Data from BFCpUEbS'!W102:W108)</f>
-        <v>1.6071705622000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W102:W108)</f>
+        <v>1.0371801717142858E-5</v>
       </c>
       <c r="X19" s="6">
-        <f>MAX('Data from BFCpUEbS'!X102:X108)</f>
-        <v>1.6162696150000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X102:X108)</f>
+        <v>1.045211385257143E-5</v>
       </c>
       <c r="Y19" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y102:Y108)</f>
-        <v>1.6231711376000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y102:Y108)</f>
+        <v>1.0522957339714288E-5</v>
       </c>
       <c r="Z19" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z102:Z108)</f>
-        <v>1.6216744626000005E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z102:Z108)</f>
+        <v>1.0564323543428573E-5</v>
       </c>
       <c r="AA19" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA102:AA108)</f>
-        <v>1.6351014882E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA102:AA108)</f>
+        <v>1.0692336163714287E-5</v>
       </c>
       <c r="AB19" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB102:AB108)</f>
-        <v>1.6222187496E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB102:AB108)</f>
+        <v>1.0691682914857144E-5</v>
       </c>
       <c r="AC19" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC102:AC108)</f>
-        <v>1.5989384384000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC102:AC108)</f>
+        <v>1.0629845330857145E-5</v>
       </c>
       <c r="AD19" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD102:AD108)</f>
-        <v>1.5812465974E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD102:AD108)</f>
+        <v>1.0639668872285715E-5</v>
       </c>
       <c r="AE19" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE102:AE108)</f>
-        <v>1.5825527034000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE102:AE108)</f>
+        <v>1.0713598545714286E-5</v>
       </c>
       <c r="AF19" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF102:AF108)</f>
-        <v>1.5860379682000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF102:AF108)</f>
+        <v>1.0777826892571429E-5</v>
       </c>
       <c r="AG19" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG102:AG108)</f>
-        <v>1.5887697314000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG102:AG108)</f>
+        <v>1.0720757907714284E-5</v>
       </c>
       <c r="AH19" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH102:AH108)</f>
-        <v>1.5869416400000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH102:AH108)</f>
+        <v>1.0704816311428572E-5</v>
       </c>
       <c r="AI19" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI102:AI108)</f>
-        <v>1.5882854028E-5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI102:AI108)</f>
+        <v>1.0757199348857141E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="6">
-        <f>MAX('Data from BFCpUEbS'!B111:B117)</f>
-        <v>1.7451800835999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B111:B117)</f>
+        <v>8.59144200857143E-6</v>
       </c>
       <c r="C20" s="6">
-        <f>MAX('Data from BFCpUEbS'!C111:C117)</f>
-        <v>1.9196885498000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C111:C117)</f>
+        <v>9.2544835922857142E-6</v>
       </c>
       <c r="D20" s="6">
-        <f>MAX('Data from BFCpUEbS'!D111:D117)</f>
-        <v>2.1466491910000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D111:D117)</f>
+        <v>9.8099847194285727E-6</v>
       </c>
       <c r="E20" s="6">
-        <f>MAX('Data from BFCpUEbS'!E111:E117)</f>
-        <v>2.2868679418000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E111:E117)</f>
+        <v>1.0005130248000001E-5</v>
       </c>
       <c r="F20" s="6">
-        <f>MAX('Data from BFCpUEbS'!F111:F117)</f>
-        <v>2.3979799969999997E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F111:F117)</f>
+        <v>1.0279154759999999E-5</v>
       </c>
       <c r="G20" s="6">
-        <f>MAX('Data from BFCpUEbS'!G111:G117)</f>
-        <v>2.5042964769999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G111:G117)</f>
+        <v>1.0639758836E-5</v>
       </c>
       <c r="H20" s="6">
-        <f>MAX('Data from BFCpUEbS'!H111:H117)</f>
-        <v>2.5908648902000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H111:H117)</f>
+        <v>1.0903829235142856E-5</v>
       </c>
       <c r="I20" s="6">
-        <f>MAX('Data from BFCpUEbS'!I111:I117)</f>
-        <v>2.6787158282000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I111:I117)</f>
+        <v>1.1227074344571429E-5</v>
       </c>
       <c r="J20" s="6">
-        <f>MAX('Data from BFCpUEbS'!J111:J117)</f>
-        <v>2.7670319008000003E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J111:J117)</f>
+        <v>1.1559476558857144E-5</v>
       </c>
       <c r="K20" s="6">
-        <f>MAX('Data from BFCpUEbS'!K111:K117)</f>
-        <v>2.8452915056000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K111:K117)</f>
+        <v>1.1827056587428572E-5</v>
       </c>
       <c r="L20" s="6">
-        <f>MAX('Data from BFCpUEbS'!L111:L117)</f>
-        <v>2.9087911071999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L111:L117)</f>
+        <v>1.2021929352285714E-5</v>
       </c>
       <c r="M20" s="6">
-        <f>MAX('Data from BFCpUEbS'!M111:M117)</f>
-        <v>2.9586269572000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M111:M117)</f>
+        <v>1.2165604929428572E-5</v>
       </c>
       <c r="N20" s="6">
-        <f>MAX('Data from BFCpUEbS'!N111:N117)</f>
-        <v>3.0045044559999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N111:N117)</f>
+        <v>1.2368060107714285E-5</v>
       </c>
       <c r="O20" s="6">
-        <f>MAX('Data from BFCpUEbS'!O111:O117)</f>
-        <v>3.0271573975999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O111:O117)</f>
+        <v>1.2417595904571429E-5</v>
       </c>
       <c r="P20" s="6">
-        <f>MAX('Data from BFCpUEbS'!P111:P117)</f>
-        <v>3.0450253664E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P111:P117)</f>
+        <v>1.2472545323428571E-5</v>
       </c>
       <c r="Q20" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q111:Q117)</f>
-        <v>3.0673179178000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q111:Q117)</f>
+        <v>1.2566910208857143E-5</v>
       </c>
       <c r="R20" s="6">
-        <f>MAX('Data from BFCpUEbS'!R111:R117)</f>
-        <v>3.0939191566000005E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R111:R117)</f>
+        <v>1.2678797127142859E-5</v>
       </c>
       <c r="S20" s="6">
-        <f>MAX('Data from BFCpUEbS'!S111:S117)</f>
-        <v>3.1213505816E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S111:S117)</f>
+        <v>1.2785257888571428E-5</v>
       </c>
       <c r="T20" s="6">
-        <f>MAX('Data from BFCpUEbS'!T111:T117)</f>
-        <v>3.1471680653999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T111:T117)</f>
+        <v>1.2877706507714286E-5</v>
       </c>
       <c r="U20" s="6">
-        <f>MAX('Data from BFCpUEbS'!U111:U117)</f>
-        <v>3.173774514E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U111:U117)</f>
+        <v>1.2978093739142857E-5</v>
       </c>
       <c r="V20" s="6">
-        <f>MAX('Data from BFCpUEbS'!V111:V117)</f>
-        <v>3.1956622548000005E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V111:V117)</f>
+        <v>1.3047566879142856E-5</v>
       </c>
       <c r="W20" s="6">
-        <f>MAX('Data from BFCpUEbS'!W111:W117)</f>
-        <v>3.2132969708000005E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W111:W117)</f>
+        <v>1.3099804198857143E-5</v>
       </c>
       <c r="X20" s="6">
-        <f>MAX('Data from BFCpUEbS'!X111:X117)</f>
-        <v>3.2294878410000004E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X111:X117)</f>
+        <v>1.3153412518571429E-5</v>
       </c>
       <c r="Y20" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y111:Y117)</f>
-        <v>3.2442282845999998E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y111:Y117)</f>
+        <v>1.3202677510285716E-5</v>
       </c>
       <c r="Z20" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z111:Z117)</f>
-        <v>3.2546553794E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z111:Z117)</f>
+        <v>1.3228862826857143E-5</v>
       </c>
       <c r="AA20" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA111:AA117)</f>
-        <v>3.2658666862000006E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA111:AA117)</f>
+        <v>1.3269446124285715E-5</v>
       </c>
       <c r="AB20" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB111:AB117)</f>
-        <v>3.2777250136000002E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB111:AB117)</f>
+        <v>1.3314191647142857E-5</v>
       </c>
       <c r="AC20" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC111:AC117)</f>
-        <v>3.2892393114000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC111:AC117)</f>
+        <v>1.3355462664285716E-5</v>
       </c>
       <c r="AD20" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD111:AD117)</f>
-        <v>3.2979921409999999E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD111:AD117)</f>
+        <v>1.3379869598000003E-5</v>
       </c>
       <c r="AE20" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE111:AE117)</f>
-        <v>3.3034483554000006E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE111:AE117)</f>
+        <v>1.3389512167428572E-5</v>
       </c>
       <c r="AF20" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF111:AF117)</f>
-        <v>3.3067066740000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF111:AF117)</f>
+        <v>1.3393029631142858E-5</v>
       </c>
       <c r="AG20" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG111:AG117)</f>
-        <v>3.3084977483999996E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG111:AG117)</f>
+        <v>1.3393540687714286E-5</v>
       </c>
       <c r="AH20" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH111:AH117)</f>
-        <v>3.3059977756000001E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH111:AH117)</f>
+        <v>1.337133662457143E-5</v>
       </c>
       <c r="AI20" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI111:AI117)</f>
-        <v>3.2981201010000001E-5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI111:AI117)</f>
+        <v>1.3325136144285714E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="11">
-        <f>MAX('Data from BFCpUEbS'!B120:B126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!B120:B126)</f>
         <v>0</v>
       </c>
       <c r="C21" s="11">
-        <f>MAX('Data from BFCpUEbS'!C120:C126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!C120:C126)</f>
         <v>0</v>
       </c>
       <c r="D21" s="11">
-        <f>MAX('Data from BFCpUEbS'!D120:D126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!D120:D126)</f>
         <v>0</v>
       </c>
       <c r="E21" s="11">
-        <f>MAX('Data from BFCpUEbS'!E120:E126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!E120:E126)</f>
         <v>0</v>
       </c>
       <c r="F21" s="11">
-        <f>MAX('Data from BFCpUEbS'!F120:F126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!F120:F126)</f>
         <v>0</v>
       </c>
       <c r="G21" s="11">
-        <f>MAX('Data from BFCpUEbS'!G120:G126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!G120:G126)</f>
         <v>0</v>
       </c>
       <c r="H21" s="11">
-        <f>MAX('Data from BFCpUEbS'!H120:H126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!H120:H126)</f>
         <v>0</v>
       </c>
       <c r="I21" s="11">
-        <f>MAX('Data from BFCpUEbS'!I120:I126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!I120:I126)</f>
         <v>0</v>
       </c>
       <c r="J21" s="11">
-        <f>MAX('Data from BFCpUEbS'!J120:J126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!J120:J126)</f>
         <v>0</v>
       </c>
       <c r="K21" s="11">
-        <f>MAX('Data from BFCpUEbS'!K120:K126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!K120:K126)</f>
         <v>0</v>
       </c>
       <c r="L21" s="11">
-        <f>MAX('Data from BFCpUEbS'!L120:L126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!L120:L126)</f>
         <v>0</v>
       </c>
       <c r="M21" s="11">
-        <f>MAX('Data from BFCpUEbS'!M120:M126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!M120:M126)</f>
         <v>0</v>
       </c>
       <c r="N21" s="11">
-        <f>MAX('Data from BFCpUEbS'!N120:N126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!N120:N126)</f>
         <v>0</v>
       </c>
       <c r="O21" s="11">
-        <f>MAX('Data from BFCpUEbS'!O120:O126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!O120:O126)</f>
         <v>0</v>
       </c>
       <c r="P21" s="11">
-        <f>MAX('Data from BFCpUEbS'!P120:P126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!P120:P126)</f>
         <v>0</v>
       </c>
       <c r="Q21" s="11">
-        <f>MAX('Data from BFCpUEbS'!Q120:Q126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!Q120:Q126)</f>
         <v>0</v>
       </c>
       <c r="R21" s="11">
-        <f>MAX('Data from BFCpUEbS'!R120:R126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!R120:R126)</f>
         <v>0</v>
       </c>
       <c r="S21" s="11">
-        <f>MAX('Data from BFCpUEbS'!S120:S126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!S120:S126)</f>
         <v>0</v>
       </c>
       <c r="T21" s="11">
-        <f>MAX('Data from BFCpUEbS'!T120:T126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!T120:T126)</f>
         <v>0</v>
       </c>
       <c r="U21" s="11">
-        <f>MAX('Data from BFCpUEbS'!U120:U126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!U120:U126)</f>
         <v>0</v>
       </c>
       <c r="V21" s="11">
-        <f>MAX('Data from BFCpUEbS'!V120:V126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!V120:V126)</f>
         <v>0</v>
       </c>
       <c r="W21" s="11">
-        <f>MAX('Data from BFCpUEbS'!W120:W126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!W120:W126)</f>
         <v>0</v>
       </c>
       <c r="X21" s="11">
-        <f>MAX('Data from BFCpUEbS'!X120:X126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!X120:X126)</f>
         <v>0</v>
       </c>
       <c r="Y21" s="11">
-        <f>MAX('Data from BFCpUEbS'!Y120:Y126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!Y120:Y126)</f>
         <v>0</v>
       </c>
       <c r="Z21" s="11">
-        <f>MAX('Data from BFCpUEbS'!Z120:Z126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!Z120:Z126)</f>
         <v>0</v>
       </c>
       <c r="AA21" s="11">
-        <f>MAX('Data from BFCpUEbS'!AA120:AA126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!AA120:AA126)</f>
         <v>0</v>
       </c>
       <c r="AB21" s="11">
-        <f>MAX('Data from BFCpUEbS'!AB120:AB126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!AB120:AB126)</f>
         <v>0</v>
       </c>
       <c r="AC21" s="11">
-        <f>MAX('Data from BFCpUEbS'!AC120:AC126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!AC120:AC126)</f>
         <v>0</v>
       </c>
       <c r="AD21" s="11">
-        <f>MAX('Data from BFCpUEbS'!AD120:AD126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!AD120:AD126)</f>
         <v>0</v>
       </c>
       <c r="AE21" s="11">
-        <f>MAX('Data from BFCpUEbS'!AE120:AE126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!AE120:AE126)</f>
         <v>0</v>
       </c>
       <c r="AF21" s="11">
-        <f>MAX('Data from BFCpUEbS'!AF120:AF126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!AF120:AF126)</f>
         <v>0</v>
       </c>
       <c r="AG21" s="11">
-        <f>MAX('Data from BFCpUEbS'!AG120:AG126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!AG120:AG126)</f>
         <v>0</v>
       </c>
       <c r="AH21" s="11">
-        <f>MAX('Data from BFCpUEbS'!AH120:AH126)</f>
+        <f>AVERAGE('Data from BFCpUEbS'!AH120:AH126)</f>
         <v>0</v>
       </c>
       <c r="AI21" s="11">
-        <f>MAX('Data from BFCpUEbS'!AI120:AI126)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI120:AI126)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
       <c r="B22" s="6">
-        <f>MAX('Data from BFCpUEbS'!B129:B135)</f>
-        <v>9.6644563917304229E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!B129:B135)</f>
+        <v>5.5225465095602419E-5</v>
       </c>
       <c r="C22" s="6">
-        <f>MAX('Data from BFCpUEbS'!C129:C135)</f>
-        <v>9.4556119540551768E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!C129:C135)</f>
+        <v>5.4032068308886725E-5</v>
       </c>
       <c r="D22" s="6">
-        <f>MAX('Data from BFCpUEbS'!D129:D135)</f>
-        <v>9.253969048713557E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!D129:D135)</f>
+        <v>5.2879823135506038E-5</v>
       </c>
       <c r="E22" s="6">
-        <f>MAX('Data from BFCpUEbS'!E129:E135)</f>
-        <v>9.0451246110383109E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!E129:E135)</f>
+        <v>5.1686426348790351E-5</v>
       </c>
       <c r="F22" s="6">
-        <f>MAX('Data from BFCpUEbS'!F129:F135)</f>
-        <v>8.8362801733630621E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!F129:F135)</f>
+        <v>5.0493029562074643E-5</v>
       </c>
       <c r="G22" s="6">
-        <f>MAX('Data from BFCpUEbS'!G129:G135)</f>
-        <v>8.6274357356878146E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!G129:G135)</f>
+        <v>4.9299632775358943E-5</v>
       </c>
       <c r="H22" s="6">
-        <f>MAX('Data from BFCpUEbS'!H129:H135)</f>
-        <v>8.4185912980125685E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!H129:H135)</f>
+        <v>4.8106235988643249E-5</v>
       </c>
       <c r="I22" s="6">
-        <f>MAX('Data from BFCpUEbS'!I129:I135)</f>
-        <v>8.2097468603373197E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!I129:I135)</f>
+        <v>4.6912839201927541E-5</v>
       </c>
       <c r="J22" s="6">
-        <f>MAX('Data from BFCpUEbS'!J129:J135)</f>
-        <v>8.0009024226620722E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!J129:J135)</f>
+        <v>4.571944241521184E-5</v>
       </c>
       <c r="K22" s="6">
-        <f>MAX('Data from BFCpUEbS'!K129:K135)</f>
-        <v>7.7949385979203577E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!K129:K135)</f>
+        <v>4.4542506273830613E-5</v>
       </c>
       <c r="L22" s="6">
-        <f>MAX('Data from BFCpUEbS'!L129:L135)</f>
-        <v>7.5870107189057208E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!L129:L135)</f>
+        <v>4.3354346965175549E-5</v>
       </c>
       <c r="M22" s="6">
-        <f>MAX('Data from BFCpUEbS'!M129:M135)</f>
-        <v>7.3790828398910853E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!M129:M135)</f>
+        <v>4.2166187656520486E-5</v>
       </c>
       <c r="N22" s="6">
-        <f>MAX('Data from BFCpUEbS'!N129:N135)</f>
-        <v>7.1711549608765337E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!N129:N135)</f>
+        <v>4.0978028347865904E-5</v>
       </c>
       <c r="O22" s="6">
-        <f>MAX('Data from BFCpUEbS'!O129:O135)</f>
-        <v>6.9632270818618968E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!O129:O135)</f>
+        <v>3.9789869039210841E-5</v>
       </c>
       <c r="P22" s="6">
-        <f>MAX('Data from BFCpUEbS'!P129:P135)</f>
-        <v>6.7552992028472613E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!P129:P135)</f>
+        <v>3.8601709730555778E-5</v>
       </c>
       <c r="Q22" s="6">
-        <f>MAX('Data from BFCpUEbS'!Q129:Q135)</f>
-        <v>6.5473713238327097E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Q129:Q135)</f>
+        <v>3.7413550421901196E-5</v>
       </c>
       <c r="R22" s="6">
-        <f>MAX('Data from BFCpUEbS'!R129:R135)</f>
-        <v>6.3394434448180728E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!R129:R135)</f>
+        <v>3.6225391113246132E-5</v>
       </c>
       <c r="S22" s="6">
-        <f>MAX('Data from BFCpUEbS'!S129:S135)</f>
-        <v>6.1315155658035213E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!S129:S135)</f>
+        <v>3.503723180459155E-5</v>
       </c>
       <c r="T22" s="6">
-        <f>MAX('Data from BFCpUEbS'!T129:T135)</f>
-        <v>5.9235876867888858E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!T129:T135)</f>
+        <v>3.3849072495936487E-5</v>
       </c>
       <c r="U22" s="6">
-        <f>MAX('Data from BFCpUEbS'!U129:U135)</f>
-        <v>5.7156598077742495E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!U129:U135)</f>
+        <v>3.2660913187281424E-5</v>
       </c>
       <c r="V22" s="6">
-        <f>MAX('Data from BFCpUEbS'!V129:V135)</f>
-        <v>5.5077319287596973E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!V129:V135)</f>
+        <v>3.1472753878626842E-5</v>
       </c>
       <c r="W22" s="6">
-        <f>MAX('Data from BFCpUEbS'!W129:W135)</f>
-        <v>5.2998040497450618E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!W129:W135)</f>
+        <v>3.0284594569971782E-5</v>
       </c>
       <c r="X22" s="6">
-        <f>MAX('Data from BFCpUEbS'!X129:X135)</f>
-        <v>5.0918761707305096E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!X129:X135)</f>
+        <v>2.9096435261317197E-5</v>
       </c>
       <c r="Y22" s="6">
-        <f>MAX('Data from BFCpUEbS'!Y129:Y135)</f>
-        <v>4.8839482917158733E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Y129:Y135)</f>
+        <v>2.7908275952662133E-5</v>
       </c>
       <c r="Z22" s="6">
-        <f>MAX('Data from BFCpUEbS'!Z129:Z135)</f>
-        <v>4.6760204127012378E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!Z129:Z135)</f>
+        <v>2.6720116644007074E-5</v>
       </c>
       <c r="AA22" s="6">
-        <f>MAX('Data from BFCpUEbS'!AA129:AA135)</f>
-        <v>4.4680925336866856E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AA129:AA135)</f>
+        <v>2.5531957335352488E-5</v>
       </c>
       <c r="AB22" s="6">
-        <f>MAX('Data from BFCpUEbS'!AB129:AB135)</f>
-        <v>4.2601646546720494E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AB129:AB135)</f>
+        <v>2.4343798026697425E-5</v>
       </c>
       <c r="AC22" s="6">
-        <f>MAX('Data from BFCpUEbS'!AC129:AC135)</f>
-        <v>4.0522367756574138E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AC129:AC135)</f>
+        <v>2.3155638718042365E-5</v>
       </c>
       <c r="AD22" s="6">
-        <f>MAX('Data from BFCpUEbS'!AD129:AD135)</f>
-        <v>3.8443088966428616E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AD129:AD135)</f>
+        <v>2.196747940938778E-5</v>
       </c>
       <c r="AE22" s="6">
-        <f>MAX('Data from BFCpUEbS'!AE129:AE135)</f>
-        <v>3.6363810176282254E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AE129:AE135)</f>
+        <v>2.0779320100732716E-5</v>
       </c>
       <c r="AF22" s="6">
-        <f>MAX('Data from BFCpUEbS'!AF129:AF135)</f>
-        <v>3.4284531386136739E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AF129:AF135)</f>
+        <v>1.9591160792078138E-5</v>
       </c>
       <c r="AG22" s="6">
-        <f>MAX('Data from BFCpUEbS'!AG129:AG135)</f>
-        <v>3.2205252595990376E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AG129:AG135)</f>
+        <v>1.8403001483423071E-5</v>
       </c>
       <c r="AH22" s="6">
-        <f>MAX('Data from BFCpUEbS'!AH129:AH135)</f>
-        <v>3.0125973805844017E-5</v>
+        <f>AVERAGE('Data from BFCpUEbS'!AH129:AH135)</f>
+        <v>1.7214842174768011E-5</v>
       </c>
       <c r="AI22" s="6">
-        <f>MAX('Data from BFCpUEbS'!AI129:AI135)</f>
-        <v>2.8046695015698495E-5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.45">
+        <f>AVERAGE('Data from BFCpUEbS'!AI129:AI135)</f>
+        <v>1.6026682866113426E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B3:AI17 B18:AI22" formulaRange="1"/>
+    <ignoredError sqref="B6:AI8 B15:AI16" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>